<commit_message>
Shay - Added additional calculations
</commit_message>
<xml_diff>
--- a/COUNTforSENGupdated.xlsx
+++ b/COUNTforSENGupdated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TonyTea/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63DD45E8-BF3F-4BA5-926C-AFE2960E1FF1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE03B33C-3671-4032-86FB-28EEF0682E7E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4780" yWindow="460" windowWidth="14400" windowHeight="16700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="114">
   <si>
     <t>re-do</t>
   </si>
@@ -108,6 +108,9 @@
     <t>s</t>
   </si>
   <si>
+    <t xml:space="preserve">% local " " " " " </t>
+  </si>
+  <si>
     <t xml:space="preserve">Wilfredo's Projects </t>
   </si>
   <si>
@@ -358,6 +361,15 @@
   </si>
   <si>
     <t>After NullFIX</t>
+  </si>
+  <si>
+    <t>% annon " " " " "</t>
+  </si>
+  <si>
+    <t>% local " " " " "</t>
+  </si>
+  <si>
+    <t>% nested + annon + local " " " " "</t>
   </si>
 </sst>
 </file>
@@ -849,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q115"/>
+  <dimension ref="A1:Q118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K99" zoomScale="58" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B115" sqref="B115:P115"/>
+    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
@@ -1340,44 +1352,46 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="15.75">
       <c r="A16" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75">
@@ -1692,38 +1706,38 @@
     </row>
     <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75">
@@ -2128,38 +2142,38 @@
     </row>
     <row r="48" spans="1:12" ht="94.5">
       <c r="A48" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15.75">
@@ -2272,7 +2286,7 @@
     </row>
     <row r="52" spans="1:12" ht="15.75">
       <c r="A52" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B52" s="5">
         <v>459</v>
@@ -2344,7 +2358,7 @@
     </row>
     <row r="54" spans="1:12" ht="15.75">
       <c r="A54" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B54" s="5">
         <v>517</v>
@@ -2380,7 +2394,7 @@
     </row>
     <row r="55" spans="1:12" ht="15.75">
       <c r="A55" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B55" s="5">
         <v>0</v>
@@ -2416,38 +2430,38 @@
     </row>
     <row r="58" spans="1:12" ht="15.75">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E58" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F58" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H58" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K58" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L58" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15.75">
@@ -2853,38 +2867,38 @@
     <row r="73" spans="1:12" ht="15.75"/>
     <row r="74" spans="1:12" ht="15.75">
       <c r="A74" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C74" s="22"/>
       <c r="D74" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L74" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="15.75">
@@ -3277,38 +3291,38 @@
     <row r="87" spans="1:12" ht="15.75"/>
     <row r="88" spans="1:12" ht="15.75">
       <c r="A88" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C88" s="22"/>
       <c r="D88" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H88" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I88" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J88" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K88" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L88" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="15.75">
@@ -3673,7 +3687,7 @@
     </row>
     <row r="99" spans="1:17" ht="15.75">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B99" s="13">
         <v>15</v>
@@ -3724,77 +3738,77 @@
     <row r="101" spans="1:17" ht="15.75"/>
     <row r="102" spans="1:17" ht="15.75">
       <c r="A102" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E102" s="20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F102" s="20"/>
       <c r="G102" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H102" s="20"/>
       <c r="I102" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K102" s="20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L102" s="20"/>
       <c r="M102" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N102" s="20"/>
       <c r="O102" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P102" s="20"/>
     </row>
     <row r="103" spans="1:17" ht="15.75">
       <c r="A103" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E103" s="21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F103" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G103" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="G103" s="21" t="s">
-        <v>108</v>
-      </c>
       <c r="H103" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="K103" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="K103" s="21" t="s">
-        <v>108</v>
-      </c>
       <c r="L103" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="M103" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="M103" s="21" t="s">
-        <v>108</v>
-      </c>
       <c r="N103" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="O103" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="O103" s="21" t="s">
-        <v>108</v>
-      </c>
       <c r="P103" s="21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q103" s="23"/>
     </row>
@@ -4300,7 +4314,7 @@
     </row>
     <row r="114" spans="1:16" ht="15.95" customHeight="1">
       <c r="A114" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C114">
         <v>4</v>
@@ -4398,6 +4412,201 @@
       <c r="P115">
         <f t="shared" si="4"/>
         <v>1.7688679245283019</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16">
+      <c r="A116" t="s">
+        <v>111</v>
+      </c>
+      <c r="B116">
+        <f>(B106/SUM(B104:B113)) * 100</f>
+        <v>2.6315789473684208</v>
+      </c>
+      <c r="C116">
+        <f t="shared" ref="C116:P116" si="5">(C106/SUM(C104:C113)) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="5"/>
+        <v>0.32040357215897475</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="5"/>
+        <v>0.32040357215897475</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="5"/>
+        <v>0.67870700563671926</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="5"/>
+        <v>0.76931909518888508</v>
+      </c>
+      <c r="I116">
+        <f t="shared" si="5"/>
+        <v>2.4030037546933665</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="5"/>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="K116">
+        <f t="shared" si="5"/>
+        <v>12.995763566673391</v>
+      </c>
+      <c r="L116">
+        <f t="shared" si="5"/>
+        <v>13.335993615323224</v>
+      </c>
+      <c r="M116">
+        <f t="shared" si="5"/>
+        <v>0.51793592940725108</v>
+      </c>
+      <c r="N116">
+        <f t="shared" si="5"/>
+        <v>0.51793592940725108</v>
+      </c>
+      <c r="O116">
+        <f t="shared" si="5"/>
+        <v>1.1894142134998513</v>
+      </c>
+      <c r="P116">
+        <f t="shared" si="5"/>
+        <v>1.3856132075471699</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16">
+      <c r="A117" t="s">
+        <v>112</v>
+      </c>
+      <c r="B117">
+        <f>(B105/SUM(B104:B113)) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <f t="shared" ref="C117:P117" si="6">(C105/SUM(C104:C113)) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K117">
+        <f t="shared" si="6"/>
+        <v>4.03469840629413E-3</v>
+      </c>
+      <c r="L117">
+        <f t="shared" si="6"/>
+        <v>3.9904229848363925E-3</v>
+      </c>
+      <c r="M117">
+        <f t="shared" si="6"/>
+        <v>0.16305390370228276</v>
+      </c>
+      <c r="N117">
+        <f t="shared" si="6"/>
+        <v>0.16305390370228276</v>
+      </c>
+      <c r="O117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16">
+      <c r="A118" t="s">
+        <v>113</v>
+      </c>
+      <c r="B118">
+        <f>SUM(B115:B117)</f>
+        <v>5.2631578947368416</v>
+      </c>
+      <c r="C118">
+        <f t="shared" ref="C118:P118" si="7">SUM(C115:C117)</f>
+        <v>1.3986013986013985</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="7"/>
+        <v>1.25</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="7"/>
+        <v>1.1861749267162043</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="7"/>
+        <v>1.1861749267162043</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="7"/>
+        <v>2.9794087196594963</v>
+      </c>
+      <c r="H118">
+        <f t="shared" si="7"/>
+        <v>3.0657940062004823</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="7"/>
+        <v>11.46433041301627</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="7"/>
+        <v>10.317460317460316</v>
+      </c>
+      <c r="K118">
+        <f t="shared" si="7"/>
+        <v>16.114585434738753</v>
+      </c>
+      <c r="L118">
+        <f t="shared" si="7"/>
+        <v>16.420590582601754</v>
+      </c>
+      <c r="M118">
+        <f t="shared" si="7"/>
+        <v>1.918281220026856</v>
+      </c>
+      <c r="N118">
+        <f t="shared" si="7"/>
+        <v>1.918281220026856</v>
+      </c>
+      <c r="O118">
+        <f t="shared" si="7"/>
+        <v>2.9735355337496285</v>
+      </c>
+      <c r="P118">
+        <f t="shared" si="7"/>
+        <v>3.154481132075472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
included median/min/max statistics for count
</commit_message>
<xml_diff>
--- a/COUNTforSENGupdated.xlsx
+++ b/COUNTforSENGupdated.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="460" windowWidth="24020" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="3400" yWindow="1180" windowWidth="20700" windowHeight="16700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="144">
   <si>
     <t>Nested type count</t>
   </si>
@@ -125,9 +125,6 @@
     <t>openCGA</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t xml:space="preserve">Logan's Projects </t>
   </si>
   <si>
@@ -435,6 +432,33 @@
   </si>
   <si>
     <t>Other Annotation count</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>% nested</t>
+  </si>
+  <si>
+    <t>% annon</t>
+  </si>
+  <si>
+    <t>% local</t>
+  </si>
+  <si>
+    <t>% nested+annon+local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX </t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIAN </t>
   </si>
 </sst>
 </file>
@@ -2023,17 +2047,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="L171" sqref="L171"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="P72" sqref="P72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.83203125" customWidth="1"/>
     <col min="2" max="11" width="15" customWidth="1"/>
+    <col min="13" max="13" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="G1" t="s">
         <v>12</v>
       </c>
@@ -2041,7 +2066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2054,7 +2079,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2067,9 +2092,9 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -2090,20 +2115,20 @@
         <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2164,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2178,7 +2203,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2217,7 +2242,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2253,7 +2278,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2289,7 +2314,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2325,7 +2350,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2365,7 +2390,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2404,8 +2429,18 @@
         <v>0</v>
       </c>
       <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M12" s="1"/>
+      <c r="N12" t="s">
+        <v>140</v>
+      </c>
+      <c r="O12" t="s">
+        <v>141</v>
+      </c>
+      <c r="P12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2445,10 +2480,22 @@
       </c>
       <c r="L13" s="1"/>
       <c r="M13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+      <c r="N13">
+        <f>MAX(B16:K16)</f>
+        <v>5.1454138702460845</v>
+      </c>
+      <c r="O13">
+        <f>MIN(B16:K16)</f>
+        <v>0.37137069547602969</v>
+      </c>
+      <c r="P13">
+        <f>MEDIAN(B16:K16)</f>
+        <v>1.2859361456226523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2485,13 +2532,43 @@
         <v>8</v>
       </c>
       <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>137</v>
+      </c>
+      <c r="N14">
+        <f>MAX(B17:L17)</f>
+        <v>1.9791967639410575</v>
+      </c>
+      <c r="O14">
+        <f>MIN(B17:K17)</f>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f>MEDIAN(B17:K17)</f>
+        <v>0.48648516330916391</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>138</v>
+      </c>
+      <c r="N15">
+        <f>MAX(B18:K18)</f>
+        <v>1.4446691707598961E-2</v>
+      </c>
+      <c r="O15">
+        <f>MIN(B18:K18)</f>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f>MEDIAN(B18:K18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2516,7 +2593,7 @@
         <v>1.8564356435643563</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f>G5/SUM(G5:G14)*100</f>
         <v>5.1454138702460845</v>
       </c>
       <c r="H16">
@@ -2535,10 +2612,25 @@
         <f t="shared" si="0"/>
         <v>0.7683073229291717</v>
       </c>
+      <c r="M16" t="s">
+        <v>139</v>
+      </c>
+      <c r="N16">
+        <f>MAX(B19:K19)</f>
+        <v>5.391498881431767</v>
+      </c>
+      <c r="O16">
+        <f>MIN(B19:K19)</f>
+        <v>0.43889264010803508</v>
+      </c>
+      <c r="P16">
+        <f>MEDIAN(B19:K19)</f>
+        <v>1.9064786913473957</v>
+      </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17">
         <f>B7/SUM(B5:B14)*100</f>
@@ -2583,7 +2675,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18">
         <f>B6/SUM(B5:B14)*100</f>
@@ -2628,7 +2720,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19">
         <f>SUM(B16:B18)</f>
@@ -2998,6 +3090,15 @@
       <c r="A33" t="s">
         <v>6</v>
       </c>
+      <c r="N33" t="s">
+        <v>135</v>
+      </c>
+      <c r="O33" t="s">
+        <v>141</v>
+      </c>
+      <c r="P33" t="s">
+        <v>143</v>
+      </c>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
     </row>
@@ -3045,10 +3146,25 @@
         <f>K23/SUM(K23:K32)*100</f>
         <v>2.0801468338941573</v>
       </c>
+      <c r="M34" t="s">
+        <v>136</v>
+      </c>
+      <c r="N34">
+        <f>MAX(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>5.3061224489795915</v>
+      </c>
+      <c r="O34">
+        <f>MIN(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>0.3710839934346678</v>
+      </c>
+      <c r="P34">
+        <f>MEDIAN(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>1.6187138577279077</v>
+      </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35">
         <f>B25/SUM(B23:B32)*100</f>
@@ -3090,10 +3206,25 @@
         <f>K25/SUM(K23:K32)*100</f>
         <v>1.2134189864382585</v>
       </c>
+      <c r="M35" t="s">
+        <v>137</v>
+      </c>
+      <c r="N35">
+        <f>MAX(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>13.317297179094686</v>
+      </c>
+      <c r="O35">
+        <f>MIN(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f>MEDIAN(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>1.5292542872662374</v>
+      </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36">
         <f>B24/SUM(B23:B32)*100</f>
@@ -3135,10 +3266,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="M36" t="s">
+        <v>138</v>
+      </c>
+      <c r="N36">
+        <f>MAX(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>2.6514649343762426E-2</v>
+      </c>
+      <c r="O36">
+        <f>MIN(Table767[#This Row])</f>
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <f>MEDIAN(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37">
         <f>SUM(B34:B36)</f>
@@ -3180,40 +3326,55 @@
         <f t="shared" si="7"/>
         <v>3.2935658203324158</v>
       </c>
+      <c r="M37" t="s">
+        <v>139</v>
+      </c>
+      <c r="N37">
+        <f>MAX(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>14.12639405204461</v>
+      </c>
+      <c r="O37">
+        <f>MIN(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>0.47455933775779635</v>
+      </c>
+      <c r="P37">
+        <f>MEDIAN(Table767[[#This Row],[Dungeon]:[Terasology]])</f>
+        <v>4.9205803135622119</v>
+      </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I39" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" t="s">
         <v>42</v>
-      </c>
-      <c r="C39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39" t="s">
-        <v>36</v>
-      </c>
-      <c r="F39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G39" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" t="s">
-        <v>39</v>
-      </c>
-      <c r="I39" t="s">
-        <v>40</v>
-      </c>
-      <c r="J39" t="s">
-        <v>41</v>
-      </c>
-      <c r="K39" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
@@ -3531,7 +3692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -3566,12 +3727,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N50" t="s">
+        <v>135</v>
+      </c>
+      <c r="O50" t="s">
+        <v>141</v>
+      </c>
+      <c r="P50" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -3615,10 +3785,25 @@
         <f t="shared" si="8"/>
         <v>1.0496671786994368E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51" t="s">
+        <v>136</v>
+      </c>
+      <c r="N51">
+        <f>MAX(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>3.434704830053667E-2</v>
+      </c>
+      <c r="O51">
+        <f>MIN(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>7.0422535211267607E-3</v>
+      </c>
+      <c r="P51">
+        <f>MEDIAN(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>1.7986073816918198E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B52">
         <f>B42/SUM(B40:B49)*100</f>
@@ -3660,10 +3845,25 @@
         <f t="shared" si="9"/>
         <v>0.24321556579621098</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52" t="s">
+        <v>137</v>
+      </c>
+      <c r="N52">
+        <f>MAX(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>4.9373881932021471</v>
+      </c>
+      <c r="O52">
+        <f>MIN(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <f>MEDIAN(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>1.0579584452343296</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B53">
         <f>B41/SUM(B40:B49)*100</f>
@@ -3705,10 +3905,25 @@
         <f>K41/SUM(K40:K49)*100</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M53" t="s">
+        <v>138</v>
+      </c>
+      <c r="N53">
+        <f>MAX(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>0.14311270125223613</v>
+      </c>
+      <c r="O53">
+        <f>MIN(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <f>MEDIAN(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B54">
         <f>SUM(B51:B53)</f>
@@ -3750,44 +3965,59 @@
         <f t="shared" si="11"/>
         <v>0.25371223758320532</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="M54" t="s">
+        <v>139</v>
+      </c>
+      <c r="N54">
+        <f>MAX(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>5.1148479427549196</v>
+      </c>
+      <c r="O54">
+        <f>MIN(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>2.0887728459530026E-2</v>
+      </c>
+      <c r="P54">
+        <f>MEDIAN(Table7679[[#This Row],[Crawler4j]:[openFire]])</f>
+        <v>1.1137118695458161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="D56" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="F56" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="G56" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="H56" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="I56" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I56" s="6" t="s">
+      <c r="J56" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J56" s="6" t="s">
+      <c r="K56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K56" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>0</v>
       </c>
@@ -3822,7 +4052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>1</v>
       </c>
@@ -3857,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>2</v>
       </c>
@@ -3892,9 +4122,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60" s="5">
         <v>459</v>
@@ -3927,7 +4157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>4</v>
       </c>
@@ -3962,9 +4192,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B62" s="5">
         <v>517</v>
@@ -3997,9 +4227,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63" s="5">
         <v>0</v>
@@ -4032,31 +4262,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>28</v>
       </c>
       <c r="B64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>29</v>
       </c>
       <c r="B65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>30</v>
       </c>
       <c r="B66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>6</v>
       </c>
       <c r="B67" s="5"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N67" t="s">
+        <v>135</v>
+      </c>
+      <c r="O67" t="s">
+        <v>141</v>
+      </c>
+      <c r="P67" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -4101,10 +4340,25 @@
         <v>0</v>
       </c>
       <c r="L68" s="5"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M68" t="s">
+        <v>136</v>
+      </c>
+      <c r="N68">
+        <f>MAX(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>8.2304526748971192</v>
+      </c>
+      <c r="O68">
+        <f>MIN(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <f>MEDIAN(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0.60971577457710069</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B69" s="5">
         <f>B59/SUM(B57:B66)*100</f>
@@ -4147,10 +4401,25 @@
         <v>0</v>
       </c>
       <c r="L69" s="5"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M69" t="s">
+        <v>137</v>
+      </c>
+      <c r="N69">
+        <f>MAX(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <f>MIN(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <f>MEDIAN(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B70">
         <f>B58/SUM(B57:B66)*100</f>
@@ -4192,10 +4461,25 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M70" t="s">
+        <v>138</v>
+      </c>
+      <c r="N70">
+        <f>MAX(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <f>MIN(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <f>MEDIAN(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B71">
         <f>SUM(B68:B70)</f>
@@ -4237,53 +4521,68 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M71" t="s">
+        <v>139</v>
+      </c>
+      <c r="N71">
+        <f>MAX(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>8.2304526748971192</v>
+      </c>
+      <c r="O71">
+        <f>MIN(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <f>MEDIAN(Table767910[[#This Row],[Quartz Scheduler]:[Hyper realistic zombie]])</f>
+        <v>0.60971577457710069</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C76" t="s">
         <v>58</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>59</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>60</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>61</v>
       </c>
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>62</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>63</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>64</v>
       </c>
-      <c r="I76" t="s">
+      <c r="J76" t="s">
         <v>65</v>
       </c>
-      <c r="J76" t="s">
+      <c r="K76" t="s">
         <v>66</v>
       </c>
-      <c r="K76" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -4318,7 +4617,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -4353,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -4388,7 +4687,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -4685,7 +4984,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B89">
         <f>(B78/SUM(B77:B86)) * 100</f>
@@ -4730,7 +5029,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B90">
         <f>(B79/SUM(B77:B86)) * 100</f>
@@ -4775,7 +5074,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B91">
         <f>SUM(B88:B90)</f>
@@ -4820,37 +5119,37 @@
     </row>
     <row r="93" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B93" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="C93" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C93" s="21" t="s">
+      <c r="D93" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D93" s="21" t="s">
+      <c r="E93" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E93" s="21" t="s">
+      <c r="F93" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F93" s="21" t="s">
+      <c r="G93" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G93" s="21" t="s">
+      <c r="H93" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="H93" s="21" t="s">
+      <c r="I93" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="I93" s="21" t="s">
+      <c r="J93" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="J93" s="21" t="s">
+      <c r="K93" s="22" t="s">
         <v>77</v>
-      </c>
-      <c r="K93" s="22" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -5262,7 +5561,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B106" s="13">
         <f>(B95/SUM(B94:B103)) * 100</f>
@@ -5307,7 +5606,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B107" s="15">
         <f>(B96/SUM(B94:B103)) * 100</f>
@@ -5352,7 +5651,7 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B108" s="23">
         <f>SUM(B105:B107)</f>
@@ -5397,37 +5696,37 @@
     </row>
     <row r="110" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C110" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="D110" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C110" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D110" s="21" t="s">
+      <c r="E110" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E110" s="21" t="s">
+      <c r="F110" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="F110" s="21" t="s">
+      <c r="G110" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G110" s="21" t="s">
+      <c r="H110" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H110" s="21" t="s">
+      <c r="I110" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I110" s="21" t="s">
+      <c r="J110" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="J110" s="21" t="s">
+      <c r="K110" s="22" t="s">
         <v>88</v>
-      </c>
-      <c r="K110" s="22" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
@@ -5782,7 +6081,7 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B121" s="13">
         <v>15</v>
@@ -5862,7 +6161,7 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B123" s="13">
         <f>B112/SUM(B111:B120)*100</f>
@@ -5907,7 +6206,7 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B124" s="13">
         <f>B113/SUM(B111:B120)*100</f>
@@ -5952,7 +6251,7 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B125" s="15">
         <f>SUM(B122:B124)</f>
@@ -5997,92 +6296,92 @@
     </row>
     <row r="127" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B127" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B127" s="20" t="s">
+      <c r="C127" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C127" s="24" t="s">
+      <c r="D127" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D127" s="21" t="s">
+      <c r="E127" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="E127" s="21" t="s">
+      <c r="F127" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="F127" s="21" t="s">
+      <c r="G127" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G127" s="21" t="s">
+      <c r="H127" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="H127" s="21" t="s">
+      <c r="I127" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="I127" s="21" t="s">
+      <c r="J127" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="J127" s="21" t="s">
+      <c r="K127" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="K127" s="21" t="s">
+      <c r="L127" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="L127" s="22" t="s">
+      <c r="M127" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="M127" s="19" t="s">
+      <c r="N127" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="N127" s="20" t="s">
+      <c r="O127" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="O127" s="24" t="s">
+      <c r="P127" s="25" t="s">
         <v>115</v>
-      </c>
-      <c r="P127" s="25" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B128" s="11"/>
       <c r="C128" s="11"/>
       <c r="D128" s="11"/>
       <c r="E128" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F128" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F128" s="27" t="s">
-        <v>119</v>
-      </c>
       <c r="G128" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="H128" s="28" t="s">
         <v>118</v>
-      </c>
-      <c r="H128" s="28" t="s">
-        <v>119</v>
       </c>
       <c r="I128" s="11"/>
       <c r="J128" s="12"/>
       <c r="K128" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="L128" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="L128" s="26" t="s">
-        <v>119</v>
-      </c>
       <c r="M128" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="N128" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="N128" s="26" t="s">
-        <v>119</v>
-      </c>
       <c r="O128" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="P128" s="30" t="s">
         <v>118</v>
-      </c>
-      <c r="P128" s="30" t="s">
-        <v>119</v>
       </c>
       <c r="Q128" s="31"/>
     </row>
@@ -6588,7 +6887,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B139" s="13"/>
       <c r="C139" s="13">
@@ -6691,7 +6990,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B141" s="13">
         <f>(B131/SUM(B129:B138)) * 100</f>
@@ -6756,7 +7055,7 @@
     </row>
     <row r="142" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B142" s="15">
         <f>(B130/SUM(B129:B138)) * 100</f>
@@ -6821,7 +7120,7 @@
     </row>
     <row r="143" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B143" s="8">
         <f>SUM(B140:B142)</f>
@@ -6902,37 +7201,37 @@
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="E146" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E146" s="1" t="s">
+      <c r="F146" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F146" s="1" t="s">
+      <c r="G146" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G146" s="1" t="s">
+      <c r="H146" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H146" s="1" t="s">
+      <c r="I146" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I146" s="1" t="s">
+      <c r="J146" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J146" s="1" t="s">
+      <c r="K146" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="K146" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
@@ -7042,7 +7341,7 @@
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B150">
         <v>51</v>
@@ -7112,7 +7411,7 @@
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B152">
         <v>93</v>
@@ -7147,7 +7446,7 @@
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -7182,7 +7481,7 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -7217,7 +7516,7 @@
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -7252,7 +7551,7 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -7332,7 +7631,7 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B158">
         <f>B148/SUM(B147:B156)*100</f>
@@ -7377,7 +7676,7 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B159">
         <f>B149/SUM(B147:B156)*100</f>
@@ -7422,7 +7721,7 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B160">
         <f>SUM(B157:B159)</f>

</xml_diff>

<commit_message>
Shay - Merged Statistics
</commit_message>
<xml_diff>
--- a/COUNTforSENGupdated.xlsx
+++ b/COUNTforSENGupdated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TonyTea/Documents/GitHub/SENG300GROUP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2194A16F-DE88-4FD7-B1D1-A9A0CB21B8FF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E6C74F9-8B70-434E-A78F-D2660A0B3DC3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4780" yWindow="460" windowWidth="24020" windowHeight="16700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="140">
   <si>
     <t>re-do</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Local Annotation</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>Other Annotation</t>
@@ -887,15 +884,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -913,11 +901,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3197,8 +3194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G56" zoomScale="58" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="M66" sqref="M66:P66"/>
+    <sheetView tabSelected="1" topLeftCell="B145" zoomScale="58" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
@@ -3210,7 +3207,7 @@
     <col min="18" max="20" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="G1" t="s">
         <v>0</v>
       </c>
@@ -3218,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="39.950000000000003" customHeight="1">
+    <row r="2" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3231,7 +3228,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3244,7 +3241,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3280,7 +3277,7 @@
       </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3316,7 +3313,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3355,7 +3352,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3394,7 +3391,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -3430,7 +3427,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3466,7 +3463,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3502,7 +3499,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3542,7 +3539,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3582,7 +3579,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3621,13 +3618,10 @@
         <v>0</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" t="s">
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>23</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -3663,14 +3657,14 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>25</v>
       </c>
       <c r="B16">
         <f>B5/SUM(B5:B14)*100</f>
@@ -3715,7 +3709,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <f>B7/SUM(B5:B14)*100</f>
@@ -3760,7 +3754,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <f>B6/SUM(B5:B14)*100</f>
@@ -3805,7 +3799,7 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <f>SUM(B16:B18)</f>
@@ -3860,37 +3854,37 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>32</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>33</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>34</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>35</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>36</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>37</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>38</v>
-      </c>
-      <c r="K22" t="s">
-        <v>39</v>
       </c>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
@@ -4166,21 +4160,21 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34">
         <f>B23/SUM(B23:B32)*100</f>
@@ -4225,7 +4219,7 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35">
         <f>B25/SUM(B23:B32)*100</f>
@@ -4270,7 +4264,7 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36">
         <f>B24/SUM(B23:B32)*100</f>
@@ -4315,7 +4309,7 @@
     </row>
     <row r="37" spans="1:18">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37">
         <f>SUM(B34:B36)</f>
@@ -4360,37 +4354,37 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>42</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>43</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>44</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>45</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>46</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>47</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>48</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>49</v>
-      </c>
-      <c r="K39" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -4710,7 +4704,7 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -4745,12 +4739,12 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51">
         <f>B40/SUM(B40:B49)</f>
@@ -4795,7 +4789,7 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B52">
         <f>B42/SUM(B40:B49)*100</f>
@@ -4840,7 +4834,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B53">
         <f>B41/SUM(B40:B49)*100</f>
@@ -4885,7 +4879,7 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B54">
         <f>SUM(B51:B53)</f>
@@ -4930,37 +4924,37 @@
     </row>
     <row r="56" spans="1:12" ht="80.099999999999994">
       <c r="A56" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="C56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="D56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="F56" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="G56" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="H56" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="I56" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I56" s="6" t="s">
+      <c r="J56" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J56" s="6" t="s">
+      <c r="K56" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="K56" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="L56" s="6"/>
     </row>
@@ -5071,7 +5065,7 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B60" s="5">
         <v>459</v>
@@ -5141,7 +5135,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="5">
         <v>517</v>
@@ -5176,7 +5170,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="5">
         <v>0</v>
@@ -5223,27 +5217,27 @@
     </row>
     <row r="66" spans="1:16" ht="15.75">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B66" s="5"/>
-      <c r="M66" s="59"/>
-      <c r="N66" s="59"/>
-      <c r="O66" s="59"/>
-      <c r="P66" s="59"/>
+      <c r="M66" s="55"/>
+      <c r="N66" s="55"/>
+      <c r="O66" s="55"/>
+      <c r="P66" s="55"/>
     </row>
     <row r="67" spans="1:16" ht="15.75">
       <c r="A67" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B67" s="5"/>
-      <c r="M67" s="41"/>
-      <c r="N67" s="59"/>
-      <c r="O67" s="59"/>
-      <c r="P67" s="59"/>
+      <c r="M67" s="38"/>
+      <c r="N67" s="55"/>
+      <c r="O67" s="55"/>
+      <c r="P67" s="55"/>
     </row>
     <row r="68" spans="1:16" ht="15.75">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B68" s="5">
         <f>B57/SUM(B57:B66)*100</f>
@@ -5286,14 +5280,14 @@
         <v>0</v>
       </c>
       <c r="L68" s="5"/>
-      <c r="M68" s="60"/>
-      <c r="N68" s="60"/>
-      <c r="O68" s="60"/>
-      <c r="P68" s="41"/>
+      <c r="M68" s="56"/>
+      <c r="N68" s="56"/>
+      <c r="O68" s="56"/>
+      <c r="P68" s="38"/>
     </row>
     <row r="69" spans="1:16">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B69" s="5">
         <f>B59/SUM(B57:B66)*100</f>
@@ -5336,14 +5330,14 @@
         <v>0</v>
       </c>
       <c r="L69" s="5"/>
-      <c r="M69" s="60"/>
-      <c r="N69" s="60"/>
-      <c r="O69" s="60"/>
+      <c r="M69" s="56"/>
+      <c r="N69" s="56"/>
+      <c r="O69" s="56"/>
       <c r="P69" s="23"/>
     </row>
     <row r="70" spans="1:16">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B70">
         <f>B58/SUM(B57:B66)*100</f>
@@ -5385,14 +5379,14 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M70" s="60"/>
-      <c r="N70" s="60"/>
-      <c r="O70" s="60"/>
+      <c r="M70" s="56"/>
+      <c r="N70" s="56"/>
+      <c r="O70" s="56"/>
       <c r="P70" s="23"/>
     </row>
     <row r="71" spans="1:16">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B71">
         <f>SUM(B68:B70)</f>
@@ -5434,9 +5428,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="M71" s="60"/>
-      <c r="N71" s="60"/>
-      <c r="O71" s="60"/>
+      <c r="M71" s="56"/>
+      <c r="N71" s="56"/>
+      <c r="O71" s="56"/>
       <c r="P71" s="23"/>
     </row>
     <row r="72" spans="1:16">
@@ -5451,37 +5445,37 @@
     </row>
     <row r="76" spans="1:16">
       <c r="A76" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C76" t="s">
         <v>66</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>67</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>68</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>69</v>
       </c>
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>70</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>71</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>72</v>
       </c>
-      <c r="I76" t="s">
+      <c r="J76" t="s">
         <v>73</v>
       </c>
-      <c r="J76" t="s">
+      <c r="K76" t="s">
         <v>74</v>
-      </c>
-      <c r="K76" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:16">
@@ -5801,7 +5795,7 @@
     </row>
     <row r="86" spans="1:16" ht="15.75">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -5833,33 +5827,33 @@
       <c r="K86">
         <v>1</v>
       </c>
-      <c r="M86" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="N86" s="58"/>
-      <c r="O86" s="58"/>
-      <c r="P86" s="58"/>
+      <c r="M86" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="N86" s="57"/>
+      <c r="O86" s="57"/>
+      <c r="P86" s="57"/>
     </row>
     <row r="87" spans="1:16" ht="15.75">
       <c r="A87" t="s">
-        <v>24</v>
-      </c>
-      <c r="M87" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M87" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="N87" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="N87" s="52" t="s">
+      <c r="O87" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="O87" s="52" t="s">
+      <c r="P87" s="53" t="s">
         <v>79</v>
-      </c>
-      <c r="P87" s="56" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="15.75">
       <c r="A88" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B88">
         <f>(B77/SUM(B77:B86)) * 100</f>
@@ -5901,23 +5895,23 @@
         <f t="shared" si="16"/>
         <v>2.7917620137299775</v>
       </c>
-      <c r="M88" s="54">
+      <c r="M88" s="51">
         <f>MAX(B88:K88)</f>
         <v>4.0816326530612246</v>
       </c>
-      <c r="N88" s="51">
+      <c r="N88" s="48">
         <f>MIN(B88:K88)</f>
         <v>1.1363636363636365</v>
       </c>
-      <c r="O88" s="51">
+      <c r="O88" s="48">
         <f>MEDIAN(B88:K88)</f>
         <v>2.8578693109585558</v>
       </c>
-      <c r="P88" s="57"/>
+      <c r="P88" s="54"/>
     </row>
     <row r="89" spans="1:16">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B89">
         <f>(B78/SUM(B77:B86)) * 100</f>
@@ -5959,23 +5953,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="M89" s="54">
+      <c r="M89" s="51">
         <f t="shared" ref="M89:M91" si="18">MAX(B89:K89)</f>
         <v>0</v>
       </c>
-      <c r="N89" s="51">
+      <c r="N89" s="48">
         <f t="shared" ref="N89:N91" si="19">MIN(B89:K89)</f>
         <v>0</v>
       </c>
-      <c r="O89" s="51">
+      <c r="O89" s="48">
         <f t="shared" ref="O89:O91" si="20">MEDIAN(B89:K89)</f>
         <v>0</v>
       </c>
-      <c r="P89" s="49"/>
+      <c r="P89" s="46"/>
     </row>
     <row r="90" spans="1:16">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B90">
         <f>(B79/SUM(B77:B86)) * 100</f>
@@ -6017,23 +6011,23 @@
         <f t="shared" si="21"/>
         <v>14.279176201372998</v>
       </c>
-      <c r="M90" s="54">
+      <c r="M90" s="51">
         <f t="shared" si="18"/>
         <v>14.279176201372998</v>
       </c>
-      <c r="N90" s="51">
+      <c r="N90" s="48">
         <f t="shared" si="19"/>
         <v>1.1363636363636365</v>
       </c>
-      <c r="O90" s="51">
+      <c r="O90" s="48">
         <f t="shared" si="20"/>
         <v>5.7217979216226365</v>
       </c>
-      <c r="P90" s="49"/>
+      <c r="P90" s="46"/>
     </row>
     <row r="91" spans="1:16">
       <c r="A91" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B91">
         <f>SUM(B88:B90)</f>
@@ -6075,53 +6069,53 @@
         <f t="shared" si="22"/>
         <v>17.070938215102977</v>
       </c>
-      <c r="M91" s="54">
+      <c r="M91" s="51">
         <f t="shared" si="18"/>
         <v>17.070938215102977</v>
       </c>
-      <c r="N91" s="51">
+      <c r="N91" s="48">
         <f t="shared" si="19"/>
         <v>2.2727272727272729</v>
       </c>
-      <c r="O91" s="51">
+      <c r="O91" s="48">
         <f t="shared" si="20"/>
         <v>8.6828596469262553</v>
       </c>
-      <c r="P91" s="50"/>
+      <c r="P91" s="47"/>
     </row>
     <row r="93" spans="1:16" ht="17.100000000000001" thickBot="1">
       <c r="A93" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B93" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="C93" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C93" s="21" t="s">
+      <c r="D93" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D93" s="21" t="s">
+      <c r="E93" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="E93" s="21" t="s">
+      <c r="F93" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="F93" s="21" t="s">
+      <c r="G93" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="G93" s="21" t="s">
+      <c r="H93" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="H93" s="21" t="s">
+      <c r="I93" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="I93" s="21" t="s">
+      <c r="J93" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="J93" s="21" t="s">
+      <c r="K93" s="22" t="s">
         <v>92</v>
-      </c>
-      <c r="K93" s="22" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:16">
@@ -6441,7 +6435,7 @@
     </row>
     <row r="103" spans="1:16" ht="15.75">
       <c r="A103" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B103" s="11">
         <v>8</v>
@@ -6473,16 +6467,16 @@
       <c r="K103" s="11">
         <v>0</v>
       </c>
-      <c r="M103" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="N103" s="58"/>
-      <c r="O103" s="58"/>
-      <c r="P103" s="58"/>
+      <c r="M103" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="N103" s="57"/>
+      <c r="O103" s="57"/>
+      <c r="P103" s="57"/>
     </row>
     <row r="104" spans="1:16" ht="15.75">
       <c r="A104" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B104" s="13"/>
       <c r="C104" s="13"/>
@@ -6491,22 +6485,22 @@
       <c r="H104" s="13"/>
       <c r="J104" s="13"/>
       <c r="K104" s="13"/>
-      <c r="M104" s="45" t="s">
+      <c r="M104" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="N104" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="N104" s="52" t="s">
+      <c r="O104" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="O104" s="52" t="s">
+      <c r="P104" s="53" t="s">
         <v>79</v>
-      </c>
-      <c r="P104" s="56" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:16" ht="15.75">
       <c r="A105" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B105" s="13">
         <f>(B94/SUM(B94:B103)) * 100</f>
@@ -6548,23 +6542,23 @@
         <f t="shared" si="23"/>
         <v>5.3406998158379375</v>
       </c>
-      <c r="M105" s="54">
+      <c r="M105" s="51">
         <f>MAX(B105:K105)</f>
         <v>15.686274509803921</v>
       </c>
-      <c r="N105" s="51">
+      <c r="N105" s="48">
         <f>MIN(B105:K105)</f>
         <v>0.32154340836012862</v>
       </c>
-      <c r="O105" s="51">
+      <c r="O105" s="48">
         <f>MEDIAN(B105:K105)</f>
         <v>3.5763280733610152</v>
       </c>
-      <c r="P105" s="57"/>
+      <c r="P105" s="54"/>
     </row>
     <row r="106" spans="1:16">
       <c r="A106" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B106" s="13">
         <f>(B95/SUM(B94:B103)) * 100</f>
@@ -6606,23 +6600,23 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="M106" s="54">
+      <c r="M106" s="51">
         <f t="shared" ref="M106:M108" si="25">MAX(B106:K106)</f>
         <v>1.5605493133583021E-2</v>
       </c>
-      <c r="N106" s="51">
+      <c r="N106" s="48">
         <f t="shared" ref="N106:N108" si="26">MIN(B106:K106)</f>
         <v>0</v>
       </c>
-      <c r="O106" s="51">
+      <c r="O106" s="48">
         <f t="shared" ref="O106:O108" si="27">MEDIAN(B106:K106)</f>
         <v>0</v>
       </c>
-      <c r="P106" s="49"/>
+      <c r="P106" s="46"/>
     </row>
     <row r="107" spans="1:16">
       <c r="A107" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B107" s="15">
         <f>(B96/SUM(B94:B103)) * 100</f>
@@ -6664,23 +6658,23 @@
         <f t="shared" si="28"/>
         <v>0.55248618784530379</v>
       </c>
-      <c r="M107" s="54">
+      <c r="M107" s="51">
         <f t="shared" si="25"/>
         <v>3.4509803921568625</v>
       </c>
-      <c r="N107" s="51">
+      <c r="N107" s="48">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="O107" s="51">
+      <c r="O107" s="48">
         <f t="shared" si="27"/>
         <v>0.50979432292499216</v>
       </c>
-      <c r="P107" s="49"/>
+      <c r="P107" s="46"/>
     </row>
     <row r="108" spans="1:16">
       <c r="A108" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B108" s="23">
         <f>SUM(B105:B107)</f>
@@ -6722,53 +6716,53 @@
         <f t="shared" si="29"/>
         <v>5.8931860036832413</v>
       </c>
-      <c r="M108" s="54">
+      <c r="M108" s="51">
         <f t="shared" si="25"/>
         <v>19.137254901960784</v>
       </c>
-      <c r="N108" s="51">
+      <c r="N108" s="48">
         <f t="shared" si="26"/>
         <v>0.61093247588424437</v>
       </c>
-      <c r="O108" s="51">
+      <c r="O108" s="48">
         <f t="shared" si="27"/>
         <v>3.7976289865774424</v>
       </c>
-      <c r="P108" s="50"/>
+      <c r="P108" s="47"/>
     </row>
     <row r="110" spans="1:16" ht="17.100000000000001" thickBot="1">
       <c r="A110" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B110" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="C110" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C110" s="21" t="s">
+      <c r="D110" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D110" s="21" t="s">
+      <c r="E110" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E110" s="21" t="s">
+      <c r="F110" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="F110" s="21" t="s">
+      <c r="G110" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="G110" s="21" t="s">
+      <c r="H110" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="H110" s="21" t="s">
+      <c r="I110" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="I110" s="21" t="s">
+      <c r="J110" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="J110" s="21" t="s">
+      <c r="K110" s="22" t="s">
         <v>103</v>
-      </c>
-      <c r="K110" s="22" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:16">
@@ -7088,7 +7082,7 @@
     </row>
     <row r="120" spans="1:17" ht="15.75">
       <c r="A120" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B120" s="11">
         <v>0</v>
@@ -7120,16 +7114,16 @@
       <c r="K120" s="11">
         <v>0</v>
       </c>
-      <c r="M120" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="N120" s="58"/>
-      <c r="O120" s="58"/>
-      <c r="P120" s="58"/>
+      <c r="M120" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="N120" s="57"/>
+      <c r="O120" s="57"/>
+      <c r="P120" s="57"/>
     </row>
     <row r="121" spans="1:17" ht="15.75">
       <c r="A121" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B121" s="13">
         <v>15</v>
@@ -7161,22 +7155,22 @@
       <c r="K121" s="13">
         <v>103</v>
       </c>
-      <c r="M121" s="45" t="s">
+      <c r="M121" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="N121" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="N121" s="52" t="s">
+      <c r="O121" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="O121" s="52" t="s">
+      <c r="P121" s="53" t="s">
         <v>79</v>
-      </c>
-      <c r="P121" s="56" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="122" spans="1:17" ht="15.75">
       <c r="A122" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B122" s="13">
         <f>B111/SUM(B111:B120)*100</f>
@@ -7218,23 +7212,23 @@
         <f t="shared" si="30"/>
         <v>0.76335877862595414</v>
       </c>
-      <c r="M122" s="54">
+      <c r="M122" s="51">
         <f>MAX(B122:K122)</f>
         <v>5.2204176334106727</v>
       </c>
-      <c r="N122" s="51">
+      <c r="N122" s="48">
         <f>MIN(B122:K122)</f>
         <v>0</v>
       </c>
-      <c r="O122" s="51">
+      <c r="O122" s="48">
         <f>MEDIAN(B122:K122)</f>
         <v>0.55232785347679958</v>
       </c>
-      <c r="P122" s="57"/>
+      <c r="P122" s="54"/>
     </row>
     <row r="123" spans="1:17">
       <c r="A123" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B123" s="13">
         <f>B112/SUM(B111:B120)*100</f>
@@ -7276,23 +7270,23 @@
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="M123" s="54">
+      <c r="M123" s="51">
         <f t="shared" ref="M123:M125" si="32">MAX(B123:K123)</f>
         <v>0</v>
       </c>
-      <c r="N123" s="51">
+      <c r="N123" s="48">
         <f t="shared" ref="N123:N125" si="33">MIN(B123:K123)</f>
         <v>0</v>
       </c>
-      <c r="O123" s="51">
+      <c r="O123" s="48">
         <f t="shared" ref="O123:O125" si="34">MEDIAN(B123:K123)</f>
         <v>0</v>
       </c>
-      <c r="P123" s="49"/>
+      <c r="P123" s="46"/>
     </row>
     <row r="124" spans="1:17">
       <c r="A124" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B124" s="13">
         <f>B113/SUM(B111:B120)*100</f>
@@ -7334,23 +7328,23 @@
         <f t="shared" si="35"/>
         <v>0.5089058524173028</v>
       </c>
-      <c r="M124" s="54">
+      <c r="M124" s="51">
         <f t="shared" si="32"/>
         <v>5.4607508532423212</v>
       </c>
-      <c r="N124" s="51">
+      <c r="N124" s="48">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="O124" s="51">
+      <c r="O124" s="48">
         <f t="shared" si="34"/>
         <v>0.86733337423563817</v>
       </c>
-      <c r="P124" s="49"/>
+      <c r="P124" s="46"/>
     </row>
     <row r="125" spans="1:17">
       <c r="A125" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B125" s="15">
         <f>SUM(B122:B124)</f>
@@ -7392,108 +7386,108 @@
         <f t="shared" si="36"/>
         <v>1.272264631043257</v>
       </c>
-      <c r="M125" s="54">
+      <c r="M125" s="51">
         <f t="shared" si="32"/>
         <v>6.8445475638051043</v>
       </c>
-      <c r="N125" s="51">
+      <c r="N125" s="48">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="O125" s="51">
+      <c r="O125" s="48">
         <f t="shared" si="34"/>
         <v>1.3732330526223655</v>
       </c>
-      <c r="P125" s="50"/>
+      <c r="P125" s="47"/>
     </row>
     <row r="127" spans="1:17" ht="17.100000000000001" thickBot="1">
       <c r="A127" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B127" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B127" s="20" t="s">
+      <c r="C127" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C127" s="24" t="s">
+      <c r="D127" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D127" s="21" t="s">
+      <c r="E127" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E127" s="21" t="s">
+      <c r="F127" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="F127" s="21" t="s">
+      <c r="G127" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="G127" s="21" t="s">
+      <c r="H127" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="H127" s="21" t="s">
+      <c r="I127" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="I127" s="21" t="s">
+      <c r="J127" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="J127" s="21" t="s">
+      <c r="K127" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="K127" s="21" t="s">
+      <c r="L127" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="L127" s="22" t="s">
+      <c r="M127" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="M127" s="19" t="s">
+      <c r="N127" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="N127" s="20" t="s">
+      <c r="O127" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="O127" s="24" t="s">
+      <c r="P127" s="25" t="s">
         <v>120</v>
-      </c>
-      <c r="P127" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="128" spans="1:17">
       <c r="A128" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B128" s="11"/>
       <c r="C128" s="11"/>
       <c r="D128" s="11"/>
       <c r="E128" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F128" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="F128" s="27" t="s">
-        <v>124</v>
-      </c>
       <c r="G128" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H128" s="28" t="s">
         <v>123</v>
-      </c>
-      <c r="H128" s="28" t="s">
-        <v>124</v>
       </c>
       <c r="I128" s="11"/>
       <c r="J128" s="12"/>
       <c r="K128" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="L128" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="L128" s="26" t="s">
-        <v>124</v>
-      </c>
       <c r="M128" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="N128" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="N128" s="26" t="s">
-        <v>124</v>
-      </c>
       <c r="O128" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="P128" s="30" t="s">
         <v>123</v>
-      </c>
-      <c r="P128" s="30" t="s">
-        <v>124</v>
       </c>
       <c r="Q128" s="31"/>
     </row>
@@ -7949,7 +7943,7 @@
     </row>
     <row r="138" spans="1:21" ht="15.95" customHeight="1">
       <c r="A138" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B138" s="13">
         <v>0</v>
@@ -7996,16 +7990,16 @@
       <c r="P138" s="33">
         <v>14</v>
       </c>
-      <c r="R138" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="S138" s="58"/>
-      <c r="T138" s="58"/>
-      <c r="U138" s="58"/>
+      <c r="R138" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="S138" s="57"/>
+      <c r="T138" s="57"/>
+      <c r="U138" s="57"/>
     </row>
     <row r="139" spans="1:21" ht="15.75">
       <c r="A139" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B139" s="13"/>
       <c r="C139" s="13">
@@ -8040,22 +8034,22 @@
         <v>142</v>
       </c>
       <c r="P139" s="33"/>
-      <c r="R139" s="45" t="s">
+      <c r="R139" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="S139" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="S139" s="52" t="s">
+      <c r="T139" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="T139" s="52" t="s">
+      <c r="U139" s="53" t="s">
         <v>79</v>
-      </c>
-      <c r="U139" s="56" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="15.75">
       <c r="A140" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B140" s="13">
         <f>(B129/SUM(B129:B138)) * 100</f>
@@ -8117,23 +8111,23 @@
         <f t="shared" si="37"/>
         <v>1.7688679245283019</v>
       </c>
-      <c r="R140" s="54">
+      <c r="R140" s="51">
         <f>MAX(B140:P140)</f>
         <v>9.0613266583229031</v>
       </c>
-      <c r="S140" s="51">
+      <c r="S140" s="48">
         <f>MIN(B140:P140)</f>
         <v>0.86577135455722953</v>
       </c>
-      <c r="T140" s="51">
+      <c r="T140" s="48">
         <f>MEDIAN(B140:P140)</f>
         <v>1.784121320249777</v>
       </c>
-      <c r="U140" s="57"/>
+      <c r="U140" s="54"/>
     </row>
     <row r="141" spans="1:21" ht="15.75">
       <c r="A141" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B141" s="13">
         <f>(B131/SUM(B129:B138)) * 100</f>
@@ -8195,23 +8189,23 @@
         <f t="shared" si="38"/>
         <v>1.3856132075471699</v>
       </c>
-      <c r="R141" s="54">
+      <c r="R141" s="51">
         <f t="shared" ref="R141:R143" si="39">MAX(B141:P141)</f>
         <v>13.335993615323224</v>
       </c>
-      <c r="S141" s="51">
+      <c r="S141" s="48">
         <f t="shared" ref="S141:S143" si="40">MIN(B141:P141)</f>
         <v>0</v>
       </c>
-      <c r="T141" s="51">
+      <c r="T141" s="48">
         <f t="shared" ref="T141:T143" si="41">MEDIAN(B141:P141)</f>
         <v>0.76931909518888508</v>
       </c>
-      <c r="U141" s="49"/>
+      <c r="U141" s="46"/>
     </row>
     <row r="142" spans="1:21" ht="17.100000000000001" thickBot="1">
       <c r="A142" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B142" s="15">
         <f>(B130/SUM(B129:B138)) * 100</f>
@@ -8273,23 +8267,23 @@
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-      <c r="R142" s="54">
+      <c r="R142" s="51">
         <f t="shared" si="39"/>
         <v>0.16305390370228276</v>
       </c>
-      <c r="S142" s="51">
+      <c r="S142" s="48">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="T142" s="51">
+      <c r="T142" s="48">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="U142" s="49"/>
+      <c r="U142" s="46"/>
     </row>
     <row r="143" spans="1:21" ht="17.100000000000001" thickBot="1">
       <c r="A143" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B143" s="8">
         <f>SUM(B140:B142)</f>
@@ -8351,19 +8345,19 @@
         <f t="shared" si="43"/>
         <v>3.154481132075472</v>
       </c>
-      <c r="R143" s="55">
+      <c r="R143" s="52">
         <f t="shared" si="39"/>
         <v>16.420590582601754</v>
       </c>
-      <c r="S143" s="53">
+      <c r="S143" s="50">
         <f t="shared" si="40"/>
         <v>1.1861749267162043</v>
       </c>
-      <c r="T143" s="53">
+      <c r="T143" s="50">
         <f t="shared" si="41"/>
         <v>2.9794087196594963</v>
       </c>
-      <c r="U143" s="50"/>
+      <c r="U143" s="47"/>
     </row>
     <row r="144" spans="1:21">
       <c r="B144" s="11"/>
@@ -8384,37 +8378,37 @@
     <row r="145" spans="1:18" ht="15.75"/>
     <row r="146" spans="1:18" ht="15.75">
       <c r="A146" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="E146" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E146" s="1" t="s">
+      <c r="F146" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F146" s="1" t="s">
+      <c r="G146" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G146" s="1" t="s">
+      <c r="H146" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H146" s="1" t="s">
+      <c r="I146" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I146" s="1" t="s">
+      <c r="J146" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="J146" s="1" t="s">
+      <c r="K146" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="K146" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="147" spans="1:18" ht="15.75">
@@ -8524,7 +8518,7 @@
     </row>
     <row r="150" spans="1:18" ht="15.75">
       <c r="A150" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B150">
         <v>51</v>
@@ -8594,7 +8588,7 @@
     </row>
     <row r="152" spans="1:18" ht="15.75">
       <c r="A152" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B152">
         <v>93</v>
@@ -8629,7 +8623,7 @@
     </row>
     <row r="153" spans="1:18" ht="15.75">
       <c r="A153" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -8664,7 +8658,7 @@
     </row>
     <row r="154" spans="1:18" ht="15.75">
       <c r="A154" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -8699,7 +8693,7 @@
     </row>
     <row r="155" spans="1:18" ht="15.75">
       <c r="A155" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -8731,16 +8725,16 @@
       <c r="K155">
         <v>0</v>
       </c>
-      <c r="M155" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="N155" s="39"/>
-      <c r="O155" s="39"/>
-      <c r="P155" s="40"/>
+      <c r="M155" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="N155" s="59"/>
+      <c r="O155" s="59"/>
+      <c r="P155" s="60"/>
     </row>
     <row r="156" spans="1:18" ht="15.75">
       <c r="A156" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -8772,23 +8766,23 @@
       <c r="K156">
         <v>0</v>
       </c>
-      <c r="M156" s="45" t="s">
+      <c r="M156" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="N156" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="N156" s="43" t="s">
+      <c r="O156" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="O156" s="43" t="s">
+      <c r="P156" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="P156" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="R156" s="42"/>
+      <c r="R156" s="39"/>
     </row>
     <row r="157" spans="1:18" ht="15.75">
       <c r="A157" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B157">
         <f>B147/SUM(B147:B156)*100</f>
@@ -8830,23 +8824,23 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="M157" s="46">
+      <c r="M157" s="43">
         <f>MAX(B157:K157)</f>
         <v>6.4837299660029144</v>
       </c>
-      <c r="N157" s="42">
+      <c r="N157" s="39">
         <f>MIN(B157:K157)</f>
         <v>0</v>
       </c>
-      <c r="O157" s="42">
+      <c r="O157" s="39">
         <f>MEDIAN(B157:K157)</f>
         <v>0.70422535211267612</v>
       </c>
-      <c r="P157" s="49"/>
+      <c r="P157" s="46"/>
     </row>
     <row r="158" spans="1:18" ht="15.75">
       <c r="A158" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B158">
         <f>B148/SUM(B147:B156)*100</f>
@@ -8888,23 +8882,23 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="M158" s="46">
+      <c r="M158" s="43">
         <f t="shared" ref="M158:M160" si="46">MAX(B158:K158)</f>
         <v>0</v>
       </c>
-      <c r="N158" s="42">
+      <c r="N158" s="39">
         <f t="shared" ref="N158:N160" si="47">MIN(B158:K158)</f>
         <v>0</v>
       </c>
-      <c r="O158" s="42">
+      <c r="O158" s="39">
         <f t="shared" ref="O158:O160" si="48">MEDIAN(B158:K158)</f>
         <v>0</v>
       </c>
-      <c r="P158" s="49"/>
+      <c r="P158" s="46"/>
     </row>
     <row r="159" spans="1:18" ht="15.75">
       <c r="A159" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B159">
         <f>B149/SUM(B147:B156)*100</f>
@@ -8946,23 +8940,23 @@
         <f t="shared" si="49"/>
         <v>2.4390243902439024</v>
       </c>
-      <c r="M159" s="46">
+      <c r="M159" s="43">
         <f t="shared" si="46"/>
         <v>6.25</v>
       </c>
-      <c r="N159" s="42">
+      <c r="N159" s="39">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="O159" s="42">
+      <c r="O159" s="39">
         <f t="shared" si="48"/>
         <v>8.5376000729477097E-2</v>
       </c>
-      <c r="P159" s="49"/>
+      <c r="P159" s="46"/>
     </row>
     <row r="160" spans="1:18" ht="15.75">
       <c r="A160" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B160">
         <f>SUM(B157:B159)</f>
@@ -9004,19 +8998,19 @@
         <f t="shared" si="50"/>
         <v>2.4390243902439024</v>
       </c>
-      <c r="M160" s="47">
+      <c r="M160" s="44">
         <f t="shared" si="46"/>
         <v>9.6163186012627495</v>
       </c>
-      <c r="N160" s="44">
+      <c r="N160" s="41">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="O160" s="44">
+      <c r="O160" s="41">
         <f t="shared" si="48"/>
         <v>2.238598095871617</v>
       </c>
-      <c r="P160" s="50"/>
+      <c r="P160" s="47"/>
     </row>
     <row r="161" spans="15:18" ht="15.75">
       <c r="O161" s="1"/>

</xml_diff>

<commit_message>
Shay - Added additional stats
</commit_message>
<xml_diff>
--- a/COUNTforSENGupdated.xlsx
+++ b/COUNTforSENGupdated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TonyTea/Documents/GitHub/SENG300GROUP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05DF951D-FC1C-4BD7-AF0B-A0AE34D6D6CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B26DDD19-37C7-408A-A23B-CE2E5A386E69}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4780" yWindow="460" windowWidth="24020" windowHeight="16700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="153">
   <si>
     <t>re-do</t>
   </si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>Results of Detailed Investigation across all projects</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -882,11 +885,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -962,19 +976,129 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="140">
+  <dxfs count="144">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -993,6 +1117,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -3660,196 +3800,196 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table46" displayName="Table46" ref="A137:P154" totalsRowShown="0" headerRowBorderDxfId="138" tableBorderDxfId="139">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table46" displayName="Table46" ref="A137:P154" totalsRowShown="0" headerRowBorderDxfId="142" tableBorderDxfId="143">
   <autoFilter ref="A137:P154" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Shay's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="BBM Secure Comms" dataDxfId="137"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="BB web samples" dataDxfId="136"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="All Algorithms" dataDxfId="135"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DeepLearning" dataDxfId="134"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column1" dataDxfId="133"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ExoPlayer" dataDxfId="132"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column2" dataDxfId="131"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dex2Java Decompiler" dataDxfId="130"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Net Cipher" dataDxfId="129"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ReactiveExtensionsForJVM" dataDxfId="128"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column3" dataDxfId="127"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="BBM Secure Comms" dataDxfId="141"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="BB web samples" dataDxfId="140"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="All Algorithms" dataDxfId="139"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DeepLearning" dataDxfId="138"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column1" dataDxfId="137"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ExoPlayer" dataDxfId="136"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column2" dataDxfId="135"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dex2Java Decompiler" dataDxfId="134"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Net Cipher" dataDxfId="133"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ReactiveExtensionsForJVM" dataDxfId="132"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column3" dataDxfId="131"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Java9 ASTParser"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column4" dataDxfId="126"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Replacement4SQLITE&amp;ORMs" dataDxfId="125"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column5" dataDxfId="124"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column4" dataDxfId="130"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Replacement4SQLITE&amp;ORMs" dataDxfId="129"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column5" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D58169DB-DE6A-4097-BB3F-6E29EBE5E4CE}" name="Table2" displayName="Table2" ref="M168:P172" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="79" tableBorderDxfId="80" totalsRowBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D58169DB-DE6A-4097-BB3F-6E29EBE5E4CE}" name="Table2" displayName="Table2" ref="M168:P172" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="83" tableBorderDxfId="84" totalsRowBorderDxfId="82">
   <autoFilter ref="M168:P172" xr:uid="{643EF349-F378-4476-861D-EB502F029625}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2F88BFBE-2BCE-4C4A-BF6C-804D0AB6C33D}" name="MAX" dataDxfId="77">
+    <tableColumn id="1" xr3:uid="{2F88BFBE-2BCE-4C4A-BF6C-804D0AB6C33D}" name="MAX" dataDxfId="81">
       <calculatedColumnFormula>MAX(B169:K169)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{957CED48-CAB2-4433-84D9-BD240400BA18}" name="MIN" dataDxfId="76">
+    <tableColumn id="2" xr3:uid="{957CED48-CAB2-4433-84D9-BD240400BA18}" name="MIN" dataDxfId="80">
       <calculatedColumnFormula>MIN(B169:K169)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2E4EE599-1FFB-4E42-84BA-EA16793515DD}" name="MEDIAN" dataDxfId="75">
+    <tableColumn id="3" xr3:uid="{2E4EE599-1FFB-4E42-84BA-EA16793515DD}" name="MEDIAN" dataDxfId="79">
       <calculatedColumnFormula>MEDIAN(B169:K169)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2F3D4A5F-CFD5-432D-A5E1-88F67A021E47}" name="OUTLIER" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{2F3D4A5F-CFD5-432D-A5E1-88F67A021E47}" name="OUTLIER" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D41C6232-F33C-4519-8651-5945885D4D09}" name="Table3" displayName="Table3" ref="R149:U153" totalsRowShown="0" headerRowDxfId="73" headerRowBorderDxfId="71" tableBorderDxfId="72" totalsRowBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D41C6232-F33C-4519-8651-5945885D4D09}" name="Table3" displayName="Table3" ref="R149:U153" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="75" tableBorderDxfId="76" totalsRowBorderDxfId="74">
   <autoFilter ref="R149:U153" xr:uid="{F7FE1993-E430-415E-90F6-18D037458B38}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5C318E04-5635-40B1-97BE-0E81731DAF67}" name="MAX" dataDxfId="69">
+    <tableColumn id="1" xr3:uid="{5C318E04-5635-40B1-97BE-0E81731DAF67}" name="MAX" dataDxfId="73">
       <calculatedColumnFormula>MAX(B150:P150)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{81E8AE5D-D4D9-4C11-ACE8-E1C1CBFC5CBB}" name="MIN" dataDxfId="68">
+    <tableColumn id="2" xr3:uid="{81E8AE5D-D4D9-4C11-ACE8-E1C1CBFC5CBB}" name="MIN" dataDxfId="72">
       <calculatedColumnFormula>MIN(B150:P150)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{07B572AF-AEDF-476D-90CA-FF6AE3BD4050}" name="MEDIAN" dataDxfId="67">
+    <tableColumn id="3" xr3:uid="{07B572AF-AEDF-476D-90CA-FF6AE3BD4050}" name="MEDIAN" dataDxfId="71">
       <calculatedColumnFormula>MEDIAN(B150:P150)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BC6D606D-23D5-4C2A-8D05-6A27A0D7C611}" name="OUTLIER" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{BC6D606D-23D5-4C2A-8D05-6A27A0D7C611}" name="OUTLIER" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CD67CC6F-B454-42FF-BAAB-DF180AB8F1FE}" name="Table35" displayName="Table35" ref="M129:P133" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="63" tableBorderDxfId="64" totalsRowBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CD67CC6F-B454-42FF-BAAB-DF180AB8F1FE}" name="Table35" displayName="Table35" ref="M129:P133" totalsRowShown="0" headerRowDxfId="69" headerRowBorderDxfId="67" tableBorderDxfId="68" totalsRowBorderDxfId="66">
   <autoFilter ref="M129:P133" xr:uid="{31727AEE-EB67-47DF-97D6-B3036D2D0919}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{59FC5E6F-3BE8-42CB-9737-6D74C506DFCE}" name="MAX" dataDxfId="61">
+    <tableColumn id="1" xr3:uid="{59FC5E6F-3BE8-42CB-9737-6D74C506DFCE}" name="MAX" dataDxfId="65">
       <calculatedColumnFormula>MAX(B130:K130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{54301EDD-72C7-4218-B7FA-A1B20F8639B9}" name="MIN" dataDxfId="60">
+    <tableColumn id="2" xr3:uid="{54301EDD-72C7-4218-B7FA-A1B20F8639B9}" name="MIN" dataDxfId="64">
       <calculatedColumnFormula>MIN(B130:K130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AE843AC-4231-4690-A69D-6E42C2A5C15F}" name="MEDIAN" dataDxfId="59">
+    <tableColumn id="3" xr3:uid="{4AE843AC-4231-4690-A69D-6E42C2A5C15F}" name="MEDIAN" dataDxfId="63">
       <calculatedColumnFormula>MEDIAN(B130:K130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3F5C3205-BCD8-4435-87FC-4DC3FC5526BF}" name="OUTLIER" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{3F5C3205-BCD8-4435-87FC-4DC3FC5526BF}" name="OUTLIER" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E89BBDFF-9BCE-41C9-A524-1C8E3D6B4E3A}" name="Table3515" displayName="Table3515" ref="M110:P114" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="55" tableBorderDxfId="56" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E89BBDFF-9BCE-41C9-A524-1C8E3D6B4E3A}" name="Table3515" displayName="Table3515" ref="M110:P114" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
   <autoFilter ref="M110:P114" xr:uid="{CD4F18DC-3DF0-4D94-8408-4AA1FE8FFA6C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F207E2EF-B246-45DD-8A6D-AD70A006F3D9}" name="MAX" dataDxfId="53">
+    <tableColumn id="1" xr3:uid="{F207E2EF-B246-45DD-8A6D-AD70A006F3D9}" name="MAX" dataDxfId="57">
       <calculatedColumnFormula>MAX(B111:K111)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C11F6B43-1EE2-42E0-9EA3-9DF4C1F96E46}" name="MIN" dataDxfId="52">
+    <tableColumn id="2" xr3:uid="{C11F6B43-1EE2-42E0-9EA3-9DF4C1F96E46}" name="MIN" dataDxfId="56">
       <calculatedColumnFormula>MIN(B111:K111)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{98D56CDE-CCEF-493F-9181-7436F54EFE2B}" name="MEDIAN" dataDxfId="51">
+    <tableColumn id="3" xr3:uid="{98D56CDE-CCEF-493F-9181-7436F54EFE2B}" name="MEDIAN" dataDxfId="55">
       <calculatedColumnFormula>MEDIAN(B111:K111)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5EB3EBF1-685F-4F48-B06E-FF03E7255773}" name="OUTLIER" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{5EB3EBF1-685F-4F48-B06E-FF03E7255773}" name="OUTLIER" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23920614-FDA3-4E4D-B401-21A03C68C443}" name="Table3516" displayName="Table3516" ref="M91:P95" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23920614-FDA3-4E4D-B401-21A03C68C443}" name="Table3516" displayName="Table3516" ref="M91:P95" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="51" tableBorderDxfId="52" totalsRowBorderDxfId="50">
   <autoFilter ref="M91:P95" xr:uid="{81A3871F-D47B-460F-8EC0-9148FA8AB78B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0026FF4C-8646-4907-928C-388F240EA8A8}" name="MAX" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{0026FF4C-8646-4907-928C-388F240EA8A8}" name="MAX" dataDxfId="49">
       <calculatedColumnFormula>MAX(B92:K92)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A10D139E-3EEE-4EE2-BFCB-596C17278338}" name="MIN" dataDxfId="44">
+    <tableColumn id="2" xr3:uid="{A10D139E-3EEE-4EE2-BFCB-596C17278338}" name="MIN" dataDxfId="48">
       <calculatedColumnFormula>MIN(B92:K92)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF9343AE-42F6-42D1-AB57-E614048687EB}" name="MEDIAN" dataDxfId="43">
+    <tableColumn id="3" xr3:uid="{EF9343AE-42F6-42D1-AB57-E614048687EB}" name="MEDIAN" dataDxfId="47">
       <calculatedColumnFormula>MEDIAN(B92:K92)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5FC9FFE9-4347-4E22-8EDB-ABFCCDCBB5A4}" name="OUTLIER" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{5FC9FFE9-4347-4E22-8EDB-ABFCCDCBB5A4}" name="OUTLIER" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5AFE4B7-E0B0-4205-95AE-602AADF7F3A2}" name="Table35162" displayName="Table35162" ref="M72:P76" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="39" tableBorderDxfId="40" totalsRowBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5AFE4B7-E0B0-4205-95AE-602AADF7F3A2}" name="Table35162" displayName="Table35162" ref="M72:P76" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="43" tableBorderDxfId="44" totalsRowBorderDxfId="42">
   <autoFilter ref="M72:P76" xr:uid="{3C82328A-A894-41F3-BCDC-160BE80C61FF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{979FB2E5-5872-45B0-8D83-5313ADB5273F}" name="MAX" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{979FB2E5-5872-45B0-8D83-5313ADB5273F}" name="MAX" dataDxfId="41">
       <calculatedColumnFormula>MAX(B73:K73)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{70F13572-BB09-4B3B-96A3-1C71C2839CB9}" name="MIN" dataDxfId="36">
+    <tableColumn id="2" xr3:uid="{70F13572-BB09-4B3B-96A3-1C71C2839CB9}" name="MIN" dataDxfId="40">
       <calculatedColumnFormula>MIN(B73:K73)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A59432C2-86B1-4456-9B70-4F7F90BA4E8B}" name="MEDIAN" dataDxfId="35">
+    <tableColumn id="3" xr3:uid="{A59432C2-86B1-4456-9B70-4F7F90BA4E8B}" name="MEDIAN" dataDxfId="39">
       <calculatedColumnFormula>MEDIAN(B73:K73)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C85B4A01-9347-4AD4-805F-F5DDC0408758}" name="OUTLIER" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{C85B4A01-9347-4AD4-805F-F5DDC0408758}" name="OUTLIER" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F33D2278-913D-4A97-82B5-44DAF92758D1}" name="Table351617" displayName="Table351617" ref="M53:P57" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="31" tableBorderDxfId="32" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F33D2278-913D-4A97-82B5-44DAF92758D1}" name="Table351617" displayName="Table351617" ref="M53:P57" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="35" tableBorderDxfId="36" totalsRowBorderDxfId="34">
   <autoFilter ref="M53:P57" xr:uid="{5AA1B32C-90CD-4CB6-ADA6-E71739CE7665}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{16772894-3593-4F23-969F-161630B58AF3}" name="MAX" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{16772894-3593-4F23-969F-161630B58AF3}" name="MAX" dataDxfId="33">
       <calculatedColumnFormula>MAX(B54:K54)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6DAE6BC6-7174-4ED5-B67A-651F35E682BE}" name="MIN" dataDxfId="28">
+    <tableColumn id="2" xr3:uid="{6DAE6BC6-7174-4ED5-B67A-651F35E682BE}" name="MIN" dataDxfId="32">
       <calculatedColumnFormula>MIN(B54:K54)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5B895D0E-1137-403E-8930-07CD754A233E}" name="MEDIAN" dataDxfId="27">
+    <tableColumn id="3" xr3:uid="{5B895D0E-1137-403E-8930-07CD754A233E}" name="MEDIAN" dataDxfId="31">
       <calculatedColumnFormula>MEDIAN(B54:K54)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{75EA28D3-E734-426B-826B-36951BA13529}" name="OUTLIER" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{75EA28D3-E734-426B-826B-36951BA13529}" name="OUTLIER" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{42728BDE-87F5-41F5-A267-B8D17A6D0EB9}" name="Table351618" displayName="Table351618" ref="M34:P38" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="23" tableBorderDxfId="24" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{42728BDE-87F5-41F5-A267-B8D17A6D0EB9}" name="Table351618" displayName="Table351618" ref="M34:P38" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="27" tableBorderDxfId="28" totalsRowBorderDxfId="26">
   <autoFilter ref="M34:P38" xr:uid="{B889D6E5-DD1F-4F42-BC04-4B45B4693F9B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F3BB2797-5CE6-42C9-9F0F-7E7A57CEE4B4}" name="MAX" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{F3BB2797-5CE6-42C9-9F0F-7E7A57CEE4B4}" name="MAX" dataDxfId="25">
       <calculatedColumnFormula>MAX(B35:K35)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5BD3DF33-103F-4395-85DC-21F888FBF2DC}" name="MIN" dataDxfId="20">
+    <tableColumn id="2" xr3:uid="{5BD3DF33-103F-4395-85DC-21F888FBF2DC}" name="MIN" dataDxfId="24">
       <calculatedColumnFormula>MIN(B35:K35)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5B130B4D-FCE8-454F-AFF4-6F934363C9F4}" name="MEDIAN" dataDxfId="19">
+    <tableColumn id="3" xr3:uid="{5B130B4D-FCE8-454F-AFF4-6F934363C9F4}" name="MEDIAN" dataDxfId="23">
       <calculatedColumnFormula>MEDIAN(B35:K35)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BF1A3C52-55FC-45CF-A141-48B2A0094A64}" name="OUTLIER" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{BF1A3C52-55FC-45CF-A141-48B2A0094A64}" name="OUTLIER" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{1A21DC82-9065-40E6-A435-4995E2233E78}" name="Table351620" displayName="Table351620" ref="M15:P19" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{1A21DC82-9065-40E6-A435-4995E2233E78}" name="Table351620" displayName="Table351620" ref="M15:P19" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
   <autoFilter ref="M15:P19" xr:uid="{1FD67088-FF9C-475B-AA9A-EF71B702AB86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2D3D5462-A43D-4F3A-A49A-3AEA69575558}" name="MAX" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{2D3D5462-A43D-4F3A-A49A-3AEA69575558}" name="MAX" dataDxfId="17">
       <calculatedColumnFormula>MAX(B16:K16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C21FA197-7971-4809-B648-BFC9865E5B57}" name="MIN" dataDxfId="12">
+    <tableColumn id="2" xr3:uid="{C21FA197-7971-4809-B648-BFC9865E5B57}" name="MIN" dataDxfId="16">
       <calculatedColumnFormula>MIN(B16:K16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C41583C2-CA8E-40C4-A961-D9964A7C6090}" name="MEDIAN" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{C41583C2-CA8E-40C4-A961-D9964A7C6090}" name="MEDIAN" dataDxfId="15">
       <calculatedColumnFormula>MEDIAN(B16:K16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{81A30073-AD6D-428B-AF86-0C95A746B0CF}" name="OUTLIER" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{81A30073-AD6D-428B-AF86-0C95A746B0CF}" name="OUTLIER" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3876,74 +4016,77 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table57" displayName="Table57" ref="A118:K133" totalsRowShown="0" headerRowDxfId="123" headerRowBorderDxfId="121" tableBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table57" displayName="Table57" ref="A118:K133" totalsRowShown="0" headerRowDxfId="127" headerRowBorderDxfId="125" tableBorderDxfId="126">
   <autoFilter ref="A118:K133" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Dal's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="GriefPrevention" dataDxfId="120"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="EssentialsX" dataDxfId="119"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="EssentialsChat" dataDxfId="118"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="WorldGuard" dataDxfId="117"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="WorldBorder" dataDxfId="116"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="PlotSquared" dataDxfId="115"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="ProtocolLib" dataDxfId="114"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="SuperVanish" dataDxfId="113"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="ViaVersion" dataDxfId="112"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="WorldEdit" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="GriefPrevention" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="EssentialsX" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="EssentialsChat" dataDxfId="122"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="WorldGuard" dataDxfId="121"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="WorldBorder" dataDxfId="120"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="PlotSquared" dataDxfId="119"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="ProtocolLib" dataDxfId="118"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="SuperVanish" dataDxfId="117"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="ViaVersion" dataDxfId="116"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="WorldEdit" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{937DC7FA-B885-4F2B-8601-8A9C7FA93035}" name="Table222" displayName="Table222" ref="M187:P191" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{937DC7FA-B885-4F2B-8601-8A9C7FA93035}" name="Table222" displayName="Table222" ref="M187:P191" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
   <autoFilter ref="M187:P191" xr:uid="{99C4CAE4-B99E-4343-B333-43A60F0E1782}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{766C641C-9FB1-4C6B-978B-806DF267ECB0}" name="MAX" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{766C641C-9FB1-4C6B-978B-806DF267ECB0}" name="MAX" dataDxfId="9">
       <calculatedColumnFormula>MAX(B188:K188)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{027B43CD-E48E-4BC3-BFC6-818B2C3C0BBB}" name="MIN" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{027B43CD-E48E-4BC3-BFC6-818B2C3C0BBB}" name="MIN" dataDxfId="8">
       <calculatedColumnFormula>MIN(B188:K188)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F47486C0-EE47-46B7-ABAC-F1671E3ECE26}" name="MEDIAN" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F47486C0-EE47-46B7-ABAC-F1671E3ECE26}" name="MEDIAN" dataDxfId="7">
       <calculatedColumnFormula>MEDIAN(B188:K188)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CE5F51EB-7E70-4060-98D3-FABE8766370E}" name="OUTLIER" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CE5F51EB-7E70-4060-98D3-FABE8766370E}" name="OUTLIER" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B4EBBF4C-6887-4930-8837-12AB03A8EF2B}" name="Table22" displayName="Table22" ref="M195:P199" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="M195:P199" xr:uid="{2813AF42-4880-4411-8CDB-B649767665D9}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A703C675-2E3B-4ECB-9A48-F5C937D8E27F}" name="MAX"/>
-    <tableColumn id="2" xr3:uid="{A4565A26-98D3-4C00-9BE3-9BD87851E4E4}" name="MIN"/>
-    <tableColumn id="3" xr3:uid="{4D259BEE-143E-4ADB-AF9B-6CE0C673BF7D}" name="MEDIAN" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B4EBBF4C-6887-4930-8837-12AB03A8EF2B}" name="Table22" displayName="Table22" ref="M195:Q199" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="M195:Q199" xr:uid="{2813AF42-4880-4411-8CDB-B649767665D9}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A703C675-2E3B-4ECB-9A48-F5C937D8E27F}" name="MAX" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A4565A26-98D3-4C00-9BE3-9BD87851E4E4}" name="MIN" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{4D259BEE-143E-4ADB-AF9B-6CE0C673BF7D}" name="MEDIAN" dataDxfId="2">
       <calculatedColumnFormula>MEDIAN(O16, O35,O54,O73,O92,O111,O130,T150,O169,O188)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3173E5D3-C27E-4C4F-AF44-4D8E0817B710}" name="OUTLIER"/>
+    <tableColumn id="4" xr3:uid="{3173E5D3-C27E-4C4F-AF44-4D8E0817B710}" name="OUTLIER" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B757222E-613A-4FE6-8E3B-A4127B80D360}" name="AVERAGE" dataDxfId="0">
+      <calculatedColumnFormula>AVERAGE(B188:K188,B169:K169,B150:P150,B130:K130,B111:K111,B111:K111,B92:K92,B73:K73,B54:K54,B35:K35,B16:K16)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table68" displayName="Table68" ref="A99:K114" totalsRowShown="0" headerRowDxfId="110" headerRowBorderDxfId="108" tableBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table68" displayName="Table68" ref="A99:K114" totalsRowShown="0" headerRowDxfId="114" headerRowBorderDxfId="112" tableBorderDxfId="113">
   <autoFilter ref="A99:K114" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Josh's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="jMonkeyEngine" dataDxfId="107"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="libGDX" dataDxfId="106"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="TEAMMATES" dataDxfId="105"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="JUnit 4" dataDxfId="104"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Activiti" dataDxfId="103"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Kore" dataDxfId="102"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="MyCollab" dataDxfId="101"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="BioJava" dataDxfId="100"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Cryptomator" dataDxfId="99"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Java Google Maps" dataDxfId="98"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="jMonkeyEngine" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="libGDX" dataDxfId="110"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="TEAMMATES" dataDxfId="109"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="JUnit 4" dataDxfId="108"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Activiti" dataDxfId="107"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Kore" dataDxfId="106"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="MyCollab" dataDxfId="105"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="BioJava" dataDxfId="104"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Cryptomator" dataDxfId="103"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Java Google Maps" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3970,7 +4113,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table76" displayName="Table76" ref="A4:K19" totalsRowShown="0" headerRowDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table76" displayName="Table76" ref="A4:K19" totalsRowShown="0" headerRowDxfId="101">
   <autoFilter ref="A4:K19" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Tony's Projects"/>
@@ -4030,11 +4173,11 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table767910" displayName="Table767910" ref="A61:K76" totalsRowShown="0" headerRowDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table767910" displayName="Table767910" ref="A61:K76" totalsRowShown="0" headerRowDxfId="100">
   <autoFilter ref="A61:K76" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Sim's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Quartz Scheduler" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Quartz Scheduler" dataDxfId="99"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Open EMRConect"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Wallet"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Secure Banking System"/>
@@ -4050,20 +4193,20 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table511" displayName="Table511" ref="A158:K172" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="92" tableBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table511" displayName="Table511" ref="A158:K172" totalsRowShown="0" headerRowDxfId="98" headerRowBorderDxfId="96" tableBorderDxfId="97">
   <autoFilter ref="A158:K172" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Robert’s Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Jpacman Framework" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="seventh" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Snake" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Java String Similarity" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="LeetCode Sol Res" dataDxfId="87"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Game of Life in Java" dataDxfId="86"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="EduMIPS64" dataDxfId="85"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="ATM Simulator" dataDxfId="84"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="RinSim" dataDxfId="83"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Mathematics" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Jpacman Framework" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="seventh" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Snake" dataDxfId="93"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Java String Similarity" dataDxfId="92"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="LeetCode Sol Res" dataDxfId="91"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Game of Life in Java" dataDxfId="90"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="EduMIPS64" dataDxfId="89"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="ATM Simulator" dataDxfId="88"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="RinSim" dataDxfId="87"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Mathematics" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4332,10 +4475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U199"/>
+  <dimension ref="A1:U200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D191" zoomScale="58" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="O200" sqref="O200"/>
+    <sheetView tabSelected="1" topLeftCell="F174" zoomScale="58" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="Q196" sqref="Q196:Q199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
@@ -4349,8 +4492,7 @@
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="15.125" customWidth="1"/>
     <col min="12" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -11235,102 +11377,124 @@
       </c>
       <c r="P191" s="46"/>
     </row>
-    <row r="193" spans="12:16" ht="15.75"/>
-    <row r="194" spans="12:16" ht="15.75">
-      <c r="M194" s="61" t="s">
+    <row r="193" spans="12:17" ht="15.75"/>
+    <row r="194" spans="12:17" ht="15.75">
+      <c r="M194" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="N194" s="61"/>
-      <c r="O194" s="61"/>
-      <c r="P194" s="61"/>
-    </row>
-    <row r="195" spans="12:16" ht="15.75">
-      <c r="M195" s="29" t="s">
+      <c r="N194" s="65"/>
+      <c r="O194" s="65"/>
+      <c r="P194" s="65"/>
+      <c r="Q194" s="66"/>
+    </row>
+    <row r="195" spans="12:17" ht="15.75">
+      <c r="M195" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="N195" s="29" t="s">
+      <c r="N195" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="O195" s="29" t="s">
+      <c r="O195" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="P195" s="29" t="s">
+      <c r="P195" s="61" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="196" spans="12:16" ht="15.75">
+      <c r="Q195" s="61" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="196" spans="12:17" ht="15.75">
       <c r="L196" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="M196">
+      <c r="M196" s="38">
         <v>15.6862745</v>
       </c>
-      <c r="N196">
-        <v>0</v>
-      </c>
-      <c r="O196">
+      <c r="N196" s="38">
+        <v>0</v>
+      </c>
+      <c r="O196" s="38">
         <f t="shared" ref="O196:O199" si="70">MEDIAN(O16, O35,O54,O73,O92,O111,O130,T150,O169,O188)</f>
         <v>1.45232500167528</v>
       </c>
-      <c r="P196">
+      <c r="P196" s="38">
         <v>3.4347049999999997E-2</v>
       </c>
-    </row>
-    <row r="197" spans="12:16" ht="15.75">
+      <c r="Q196" s="38">
+        <f>AVERAGE(B188:K188,B169:K169,B150:P150,B130:K130,B111:K111,B111:K111,B92:K92,B73:K73,B54:K54,B35:K35,B16:K16)</f>
+        <v>2.2961292895796741</v>
+      </c>
+    </row>
+    <row r="197" spans="12:17" ht="15.75">
       <c r="L197" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="M197">
+      <c r="M197" s="38">
         <v>13.3359936</v>
       </c>
-      <c r="N197">
-        <v>0</v>
-      </c>
-      <c r="O197">
+      <c r="N197" s="38">
+        <v>0</v>
+      </c>
+      <c r="O197" s="38">
         <f t="shared" si="70"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="12:16" ht="15.75">
+      <c r="P197" s="38"/>
+      <c r="Q197" s="38">
+        <f t="shared" ref="Q197:Q199" si="71">AVERAGE(B189:K189,B170:K170,B151:P151,B131:K131,B112:K112,B112:K112,B93:K93,B74:K74,B55:K55,B36:K36,B17:K17)</f>
+        <v>0.83441732142533187</v>
+      </c>
+    </row>
+    <row r="198" spans="12:17" ht="15.75">
       <c r="L198" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="M198">
+      <c r="M198" s="38">
         <v>14.2791762</v>
       </c>
-      <c r="N198">
-        <v>0</v>
-      </c>
-      <c r="O198">
+      <c r="N198" s="38">
+        <v>0</v>
+      </c>
+      <c r="O198" s="38">
         <f t="shared" si="70"/>
         <v>4.2688000364738549E-2</v>
       </c>
-      <c r="P198">
+      <c r="P198" s="38">
         <v>14.2791762</v>
       </c>
-    </row>
-    <row r="199" spans="12:16" ht="15.75">
-      <c r="L199" s="64" t="s">
+      <c r="Q198" s="38">
+        <f t="shared" si="71"/>
+        <v>1.1588949501015127</v>
+      </c>
+    </row>
+    <row r="199" spans="12:17" ht="15.75">
+      <c r="L199" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="M199">
+      <c r="M199" s="38">
         <v>19.137254899999999</v>
       </c>
-      <c r="N199">
-        <v>0</v>
-      </c>
-      <c r="O199">
+      <c r="N199" s="38">
+        <v>0</v>
+      </c>
+      <c r="O199" s="38">
         <f t="shared" si="70"/>
         <v>2.6090034077655568</v>
       </c>
-      <c r="P199">
+      <c r="P199" s="38">
         <v>17.070938200000001</v>
       </c>
-    </row>
+      <c r="Q199" s="38">
+        <f t="shared" si="71"/>
+        <v>4.289441561106516</v>
+      </c>
+    </row>
+    <row r="200" spans="12:17" ht="15.75"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="M186:P186"/>
-    <mergeCell ref="M194:P194"/>
+    <mergeCell ref="M194:Q194"/>
     <mergeCell ref="M71:P71"/>
     <mergeCell ref="M52:P52"/>
     <mergeCell ref="M33:P33"/>

</xml_diff>

<commit_message>
Removed Import declarations. from excel
</commit_message>
<xml_diff>
--- a/COUNTforSENGupdated.xlsx
+++ b/COUNTforSENGupdated.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TonyTea/Documents/GitHub/SENG300GROUP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B26DDD19-37C7-408A-A23B-CE2E5A386E69}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="460" windowWidth="24020" windowHeight="16700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4780" yWindow="460" windowWidth="24020" windowHeight="16700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179016" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,13 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="153">
-  <si>
-    <t>re-do</t>
-  </si>
-  <si>
-    <t>changed annot</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="150">
   <si>
     <t>Tony's Projects</t>
   </si>
@@ -87,9 +80,6 @@
     <t>Marker Annotation</t>
   </si>
   <si>
-    <t>Import Declr</t>
-  </si>
-  <si>
     <t>Nested Annotation</t>
   </si>
   <si>
@@ -234,9 +224,6 @@
     <t>Annotation type Count</t>
   </si>
   <si>
-    <t>Import Declarations Count</t>
-  </si>
-  <si>
     <t>Amy's Projects</t>
   </si>
   <si>
@@ -487,13 +474,16 @@
   </si>
   <si>
     <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>Import Declarations NOT used for analysis, so not counted. We are interested in the Java TYPES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -780,52 +770,52 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -834,7 +824,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -842,10 +832,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -853,23 +843,23 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -889,10 +879,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -962,9 +952,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -974,11 +966,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -986,6 +973,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1114,7 +1104,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border>
@@ -1227,13 +1216,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1243,6 +1225,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1262,7 +1251,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border>
@@ -1316,7 +1304,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1354,7 +1341,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1392,7 +1378,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1423,13 +1408,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1439,6 +1417,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1458,7 +1443,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1513,7 +1497,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1551,7 +1534,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1589,7 +1571,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1620,13 +1601,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1636,6 +1610,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1655,7 +1636,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1710,7 +1690,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1748,7 +1727,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1786,7 +1764,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1817,13 +1794,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1833,6 +1803,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1852,7 +1829,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1907,7 +1883,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1945,7 +1920,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1983,7 +1957,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2014,13 +1987,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2030,6 +1996,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2049,7 +2022,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2104,7 +2076,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2142,7 +2113,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2180,7 +2150,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2211,13 +2180,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2227,6 +2189,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2246,7 +2215,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2301,7 +2269,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2339,7 +2306,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2377,7 +2343,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2408,13 +2373,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2424,6 +2382,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2443,7 +2408,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2498,7 +2462,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2536,7 +2499,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2574,7 +2536,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2605,13 +2566,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2621,6 +2575,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2640,7 +2601,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2695,7 +2655,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2733,7 +2692,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2771,7 +2729,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2802,13 +2759,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2818,6 +2768,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2837,7 +2794,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2951,13 +2907,6 @@
     </dxf>
     <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2967,6 +2916,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2986,7 +2942,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border>
@@ -3148,16 +3103,16 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -3357,16 +3312,16 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -3523,16 +3478,16 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -3771,19 +3726,19 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <right style="thin">
           <color auto="1"/>
         </right>
         <top style="medium">
           <color auto="1"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -3800,271 +3755,271 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table46" displayName="Table46" ref="A137:P154" totalsRowShown="0" headerRowBorderDxfId="142" tableBorderDxfId="143">
-  <autoFilter ref="A137:P154" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table46" displayName="Table46" ref="A137:P154" totalsRowShown="0" headerRowBorderDxfId="143" tableBorderDxfId="142">
+  <autoFilter ref="A137:P154"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Shay's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="BBM Secure Comms" dataDxfId="141"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="BB web samples" dataDxfId="140"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="All Algorithms" dataDxfId="139"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DeepLearning" dataDxfId="138"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column1" dataDxfId="137"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ExoPlayer" dataDxfId="136"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column2" dataDxfId="135"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dex2Java Decompiler" dataDxfId="134"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Net Cipher" dataDxfId="133"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ReactiveExtensionsForJVM" dataDxfId="132"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column3" dataDxfId="131"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Java9 ASTParser"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column4" dataDxfId="130"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Replacement4SQLITE&amp;ORMs" dataDxfId="129"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column5" dataDxfId="128"/>
+    <tableColumn id="1" name="Shay's Projects"/>
+    <tableColumn id="2" name="BBM Secure Comms" dataDxfId="141"/>
+    <tableColumn id="3" name="BB web samples" dataDxfId="140"/>
+    <tableColumn id="4" name="All Algorithms" dataDxfId="139"/>
+    <tableColumn id="5" name="DeepLearning" dataDxfId="138"/>
+    <tableColumn id="6" name="Column1" dataDxfId="137"/>
+    <tableColumn id="7" name="ExoPlayer" dataDxfId="136"/>
+    <tableColumn id="8" name="Column2" dataDxfId="135"/>
+    <tableColumn id="9" name="Dex2Java Decompiler" dataDxfId="134"/>
+    <tableColumn id="10" name="Net Cipher" dataDxfId="133"/>
+    <tableColumn id="11" name="ReactiveExtensionsForJVM" dataDxfId="132"/>
+    <tableColumn id="12" name="Column3" dataDxfId="131"/>
+    <tableColumn id="13" name="Java9 ASTParser"/>
+    <tableColumn id="14" name="Column4" dataDxfId="130"/>
+    <tableColumn id="15" name="Replacement4SQLITE&amp;ORMs" dataDxfId="129"/>
+    <tableColumn id="16" name="Column5" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D58169DB-DE6A-4097-BB3F-6E29EBE5E4CE}" name="Table2" displayName="Table2" ref="M168:P172" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="83" tableBorderDxfId="84" totalsRowBorderDxfId="82">
-  <autoFilter ref="M168:P172" xr:uid="{643EF349-F378-4476-861D-EB502F029625}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="M168:P172" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="84" tableBorderDxfId="83" totalsRowBorderDxfId="82">
+  <autoFilter ref="M168:P172"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2F88BFBE-2BCE-4C4A-BF6C-804D0AB6C33D}" name="MAX" dataDxfId="81">
+    <tableColumn id="1" name="MAX" dataDxfId="81">
       <calculatedColumnFormula>MAX(B169:K169)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{957CED48-CAB2-4433-84D9-BD240400BA18}" name="MIN" dataDxfId="80">
+    <tableColumn id="2" name="MIN" dataDxfId="80">
       <calculatedColumnFormula>MIN(B169:K169)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2E4EE599-1FFB-4E42-84BA-EA16793515DD}" name="MEDIAN" dataDxfId="79">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="79">
       <calculatedColumnFormula>MEDIAN(B169:K169)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2F3D4A5F-CFD5-432D-A5E1-88F67A021E47}" name="OUTLIER" dataDxfId="78"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D41C6232-F33C-4519-8651-5945885D4D09}" name="Table3" displayName="Table3" ref="R149:U153" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="75" tableBorderDxfId="76" totalsRowBorderDxfId="74">
-  <autoFilter ref="R149:U153" xr:uid="{F7FE1993-E430-415E-90F6-18D037458B38}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="R149:U153" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75" totalsRowBorderDxfId="74">
+  <autoFilter ref="R149:U153"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5C318E04-5635-40B1-97BE-0E81731DAF67}" name="MAX" dataDxfId="73">
+    <tableColumn id="1" name="MAX" dataDxfId="73">
       <calculatedColumnFormula>MAX(B150:P150)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{81E8AE5D-D4D9-4C11-ACE8-E1C1CBFC5CBB}" name="MIN" dataDxfId="72">
+    <tableColumn id="2" name="MIN" dataDxfId="72">
       <calculatedColumnFormula>MIN(B150:P150)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{07B572AF-AEDF-476D-90CA-FF6AE3BD4050}" name="MEDIAN" dataDxfId="71">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="71">
       <calculatedColumnFormula>MEDIAN(B150:P150)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BC6D606D-23D5-4C2A-8D05-6A27A0D7C611}" name="OUTLIER" dataDxfId="70"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CD67CC6F-B454-42FF-BAAB-DF180AB8F1FE}" name="Table35" displayName="Table35" ref="M129:P133" totalsRowShown="0" headerRowDxfId="69" headerRowBorderDxfId="67" tableBorderDxfId="68" totalsRowBorderDxfId="66">
-  <autoFilter ref="M129:P133" xr:uid="{31727AEE-EB67-47DF-97D6-B3036D2D0919}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="M129:P133" totalsRowShown="0" headerRowDxfId="69" headerRowBorderDxfId="68" tableBorderDxfId="67" totalsRowBorderDxfId="66">
+  <autoFilter ref="M129:P133"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{59FC5E6F-3BE8-42CB-9737-6D74C506DFCE}" name="MAX" dataDxfId="65">
+    <tableColumn id="1" name="MAX" dataDxfId="65">
       <calculatedColumnFormula>MAX(B130:K130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{54301EDD-72C7-4218-B7FA-A1B20F8639B9}" name="MIN" dataDxfId="64">
+    <tableColumn id="2" name="MIN" dataDxfId="64">
       <calculatedColumnFormula>MIN(B130:K130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AE843AC-4231-4690-A69D-6E42C2A5C15F}" name="MEDIAN" dataDxfId="63">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="63">
       <calculatedColumnFormula>MEDIAN(B130:K130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3F5C3205-BCD8-4435-87FC-4DC3FC5526BF}" name="OUTLIER" dataDxfId="62"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E89BBDFF-9BCE-41C9-A524-1C8E3D6B4E3A}" name="Table3515" displayName="Table3515" ref="M110:P114" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
-  <autoFilter ref="M110:P114" xr:uid="{CD4F18DC-3DF0-4D94-8408-4AA1FE8FFA6C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table3515" displayName="Table3515" ref="M110:P114" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+  <autoFilter ref="M110:P114"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F207E2EF-B246-45DD-8A6D-AD70A006F3D9}" name="MAX" dataDxfId="57">
+    <tableColumn id="1" name="MAX" dataDxfId="57">
       <calculatedColumnFormula>MAX(B111:K111)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C11F6B43-1EE2-42E0-9EA3-9DF4C1F96E46}" name="MIN" dataDxfId="56">
+    <tableColumn id="2" name="MIN" dataDxfId="56">
       <calculatedColumnFormula>MIN(B111:K111)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{98D56CDE-CCEF-493F-9181-7436F54EFE2B}" name="MEDIAN" dataDxfId="55">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="55">
       <calculatedColumnFormula>MEDIAN(B111:K111)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5EB3EBF1-685F-4F48-B06E-FF03E7255773}" name="OUTLIER" dataDxfId="54"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23920614-FDA3-4E4D-B401-21A03C68C443}" name="Table3516" displayName="Table3516" ref="M91:P95" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="51" tableBorderDxfId="52" totalsRowBorderDxfId="50">
-  <autoFilter ref="M91:P95" xr:uid="{81A3871F-D47B-460F-8EC0-9148FA8AB78B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table3516" displayName="Table3516" ref="M91:P95" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+  <autoFilter ref="M91:P95"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0026FF4C-8646-4907-928C-388F240EA8A8}" name="MAX" dataDxfId="49">
+    <tableColumn id="1" name="MAX" dataDxfId="49">
       <calculatedColumnFormula>MAX(B92:K92)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A10D139E-3EEE-4EE2-BFCB-596C17278338}" name="MIN" dataDxfId="48">
+    <tableColumn id="2" name="MIN" dataDxfId="48">
       <calculatedColumnFormula>MIN(B92:K92)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF9343AE-42F6-42D1-AB57-E614048687EB}" name="MEDIAN" dataDxfId="47">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="47">
       <calculatedColumnFormula>MEDIAN(B92:K92)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5FC9FFE9-4347-4E22-8EDB-ABFCCDCBB5A4}" name="OUTLIER" dataDxfId="46"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5AFE4B7-E0B0-4205-95AE-602AADF7F3A2}" name="Table35162" displayName="Table35162" ref="M72:P76" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="43" tableBorderDxfId="44" totalsRowBorderDxfId="42">
-  <autoFilter ref="M72:P76" xr:uid="{3C82328A-A894-41F3-BCDC-160BE80C61FF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table35162" displayName="Table35162" ref="M72:P76" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="M72:P76"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{979FB2E5-5872-45B0-8D83-5313ADB5273F}" name="MAX" dataDxfId="41">
+    <tableColumn id="1" name="MAX" dataDxfId="41">
       <calculatedColumnFormula>MAX(B73:K73)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{70F13572-BB09-4B3B-96A3-1C71C2839CB9}" name="MIN" dataDxfId="40">
+    <tableColumn id="2" name="MIN" dataDxfId="40">
       <calculatedColumnFormula>MIN(B73:K73)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A59432C2-86B1-4456-9B70-4F7F90BA4E8B}" name="MEDIAN" dataDxfId="39">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="39">
       <calculatedColumnFormula>MEDIAN(B73:K73)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C85B4A01-9347-4AD4-805F-F5DDC0408758}" name="OUTLIER" dataDxfId="38"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F33D2278-913D-4A97-82B5-44DAF92758D1}" name="Table351617" displayName="Table351617" ref="M53:P57" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="35" tableBorderDxfId="36" totalsRowBorderDxfId="34">
-  <autoFilter ref="M53:P57" xr:uid="{5AA1B32C-90CD-4CB6-ADA6-E71739CE7665}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table351617" displayName="Table351617" ref="M53:P57" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="M53:P57"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{16772894-3593-4F23-969F-161630B58AF3}" name="MAX" dataDxfId="33">
+    <tableColumn id="1" name="MAX" dataDxfId="33">
       <calculatedColumnFormula>MAX(B54:K54)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6DAE6BC6-7174-4ED5-B67A-651F35E682BE}" name="MIN" dataDxfId="32">
+    <tableColumn id="2" name="MIN" dataDxfId="32">
       <calculatedColumnFormula>MIN(B54:K54)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5B895D0E-1137-403E-8930-07CD754A233E}" name="MEDIAN" dataDxfId="31">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="31">
       <calculatedColumnFormula>MEDIAN(B54:K54)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{75EA28D3-E734-426B-826B-36951BA13529}" name="OUTLIER" dataDxfId="30"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{42728BDE-87F5-41F5-A267-B8D17A6D0EB9}" name="Table351618" displayName="Table351618" ref="M34:P38" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="27" tableBorderDxfId="28" totalsRowBorderDxfId="26">
-  <autoFilter ref="M34:P38" xr:uid="{B889D6E5-DD1F-4F42-BC04-4B45B4693F9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table351618" displayName="Table351618" ref="M34:P38" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="M34:P38"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F3BB2797-5CE6-42C9-9F0F-7E7A57CEE4B4}" name="MAX" dataDxfId="25">
+    <tableColumn id="1" name="MAX" dataDxfId="25">
       <calculatedColumnFormula>MAX(B35:K35)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5BD3DF33-103F-4395-85DC-21F888FBF2DC}" name="MIN" dataDxfId="24">
+    <tableColumn id="2" name="MIN" dataDxfId="24">
       <calculatedColumnFormula>MIN(B35:K35)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5B130B4D-FCE8-454F-AFF4-6F934363C9F4}" name="MEDIAN" dataDxfId="23">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="23">
       <calculatedColumnFormula>MEDIAN(B35:K35)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BF1A3C52-55FC-45CF-A141-48B2A0094A64}" name="OUTLIER" dataDxfId="22"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{1A21DC82-9065-40E6-A435-4995E2233E78}" name="Table351620" displayName="Table351620" ref="M15:P19" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
-  <autoFilter ref="M15:P19" xr:uid="{1FD67088-FF9C-475B-AA9A-EF71B702AB86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table351620" displayName="Table351620" ref="M15:P19" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="M15:P19"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2D3D5462-A43D-4F3A-A49A-3AEA69575558}" name="MAX" dataDxfId="17">
+    <tableColumn id="1" name="MAX" dataDxfId="17">
       <calculatedColumnFormula>MAX(B16:K16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C21FA197-7971-4809-B648-BFC9865E5B57}" name="MIN" dataDxfId="16">
+    <tableColumn id="2" name="MIN" dataDxfId="16">
       <calculatedColumnFormula>MIN(B16:K16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C41583C2-CA8E-40C4-A961-D9964A7C6090}" name="MEDIAN" dataDxfId="15">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="15">
       <calculatedColumnFormula>MEDIAN(B16:K16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{81A30073-AD6D-428B-AF86-0C95A746B0CF}" name="OUTLIER" dataDxfId="14"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{08C86BB0-1F61-471E-BF2A-989001F44AFA}" name="Table20" displayName="Table20" ref="A176:K191" totalsRowShown="0">
-  <autoFilter ref="A176:K191" xr:uid="{17EF61F2-7C7D-43B8-ABEC-73DF4DB3EF6A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A176:K191" totalsRowShown="0">
+  <autoFilter ref="A176:K191"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7BD7AB6B-11D0-452B-9901-A54D03F1638A}" name="Jin's Projects"/>
-    <tableColumn id="2" xr3:uid="{82D0D090-D5BD-4B9A-8EC2-1792B624993A}" name="cSploit"/>
-    <tableColumn id="3" xr3:uid="{CC122103-1887-4D63-A17A-8024AD953D65}" name="SecurityShepherd"/>
-    <tableColumn id="4" xr3:uid="{5CF60244-0974-4A4B-A351-5D1046D39019}" name="Zuul"/>
-    <tableColumn id="5" xr3:uid="{A9A7D68A-5ADF-4FC2-BF0A-5A08195615F5}" name="SearchGuard"/>
-    <tableColumn id="6" xr3:uid="{E4E3543C-5354-4CC8-A1AF-27D151604492}" name="Pac4j"/>
-    <tableColumn id="7" xr3:uid="{3B3A8455-703A-423F-9E83-2F795F69EE2E}" name="Hive2Hive"/>
-    <tableColumn id="8" xr3:uid="{98C1F772-B122-411E-AF62-0290E80C3965}" name="Shuttle Music Player"/>
-    <tableColumn id="9" xr3:uid="{08F8C364-CCAE-416F-98E1-789165EBAA30}" name="Stylish Music Player"/>
-    <tableColumn id="10" xr3:uid="{9808EF10-1B3C-4EF4-8C51-E420EECC043B}" name="WhorlWind"/>
-    <tableColumn id="11" xr3:uid="{104175CC-3AD2-48C5-87A4-2FB23F3F2EA8}" name="Cryptopmater"/>
+    <tableColumn id="1" name="Jin's Projects"/>
+    <tableColumn id="2" name="cSploit"/>
+    <tableColumn id="3" name="SecurityShepherd"/>
+    <tableColumn id="4" name="Zuul"/>
+    <tableColumn id="5" name="SearchGuard"/>
+    <tableColumn id="6" name="Pac4j"/>
+    <tableColumn id="7" name="Hive2Hive"/>
+    <tableColumn id="8" name="Shuttle Music Player"/>
+    <tableColumn id="9" name="Stylish Music Player"/>
+    <tableColumn id="10" name="WhorlWind"/>
+    <tableColumn id="11" name="Cryptopmater"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table57" displayName="Table57" ref="A118:K133" totalsRowShown="0" headerRowDxfId="127" headerRowBorderDxfId="125" tableBorderDxfId="126">
-  <autoFilter ref="A118:K133" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="A118:K133" totalsRowShown="0" headerRowDxfId="127" headerRowBorderDxfId="126" tableBorderDxfId="125">
+  <autoFilter ref="A118:K133"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Dal's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="GriefPrevention" dataDxfId="124"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="EssentialsX" dataDxfId="123"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="EssentialsChat" dataDxfId="122"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="WorldGuard" dataDxfId="121"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="WorldBorder" dataDxfId="120"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="PlotSquared" dataDxfId="119"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="ProtocolLib" dataDxfId="118"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="SuperVanish" dataDxfId="117"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="ViaVersion" dataDxfId="116"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="WorldEdit" dataDxfId="115"/>
+    <tableColumn id="1" name="Dal's Projects"/>
+    <tableColumn id="2" name="GriefPrevention" dataDxfId="124"/>
+    <tableColumn id="4" name="EssentialsX" dataDxfId="123"/>
+    <tableColumn id="5" name="EssentialsChat" dataDxfId="122"/>
+    <tableColumn id="6" name="WorldGuard" dataDxfId="121"/>
+    <tableColumn id="7" name="WorldBorder" dataDxfId="120"/>
+    <tableColumn id="8" name="PlotSquared" dataDxfId="119"/>
+    <tableColumn id="9" name="ProtocolLib" dataDxfId="118"/>
+    <tableColumn id="10" name="SuperVanish" dataDxfId="117"/>
+    <tableColumn id="11" name="ViaVersion" dataDxfId="116"/>
+    <tableColumn id="12" name="WorldEdit" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{937DC7FA-B885-4F2B-8601-8A9C7FA93035}" name="Table222" displayName="Table222" ref="M187:P191" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
-  <autoFilter ref="M187:P191" xr:uid="{99C4CAE4-B99E-4343-B333-43A60F0E1782}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table222" displayName="Table222" ref="M187:P191" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="M187:P191"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{766C641C-9FB1-4C6B-978B-806DF267ECB0}" name="MAX" dataDxfId="9">
+    <tableColumn id="1" name="MAX" dataDxfId="9">
       <calculatedColumnFormula>MAX(B188:K188)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{027B43CD-E48E-4BC3-BFC6-818B2C3C0BBB}" name="MIN" dataDxfId="8">
+    <tableColumn id="2" name="MIN" dataDxfId="8">
       <calculatedColumnFormula>MIN(B188:K188)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F47486C0-EE47-46B7-ABAC-F1671E3ECE26}" name="MEDIAN" dataDxfId="7">
+    <tableColumn id="3" name="MEDIAN" dataDxfId="7">
       <calculatedColumnFormula>MEDIAN(B188:K188)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CE5F51EB-7E70-4060-98D3-FABE8766370E}" name="OUTLIER" dataDxfId="6"/>
+    <tableColumn id="4" name="OUTLIER" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B4EBBF4C-6887-4930-8837-12AB03A8EF2B}" name="Table22" displayName="Table22" ref="M195:Q199" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="M195:Q199" xr:uid="{2813AF42-4880-4411-8CDB-B649767665D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="M195:Q199" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="M195:Q199"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A703C675-2E3B-4ECB-9A48-F5C937D8E27F}" name="MAX" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A4565A26-98D3-4C00-9BE3-9BD87851E4E4}" name="MIN" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{4D259BEE-143E-4ADB-AF9B-6CE0C673BF7D}" name="MEDIAN" dataDxfId="2">
+    <tableColumn id="1" name="MAX" dataDxfId="4"/>
+    <tableColumn id="2" name="MIN" dataDxfId="3"/>
+    <tableColumn id="3" name="MEDIAN" dataDxfId="2">
       <calculatedColumnFormula>MEDIAN(O16, O35,O54,O73,O92,O111,O130,T150,O169,O188)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3173E5D3-C27E-4C4F-AF44-4D8E0817B710}" name="OUTLIER" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{B757222E-613A-4FE6-8E3B-A4127B80D360}" name="AVERAGE" dataDxfId="0">
+    <tableColumn id="4" name="OUTLIER" dataDxfId="1"/>
+    <tableColumn id="5" name="AVERAGE" dataDxfId="0">
       <calculatedColumnFormula>AVERAGE(B188:K188,B169:K169,B150:P150,B130:K130,B111:K111,B111:K111,B92:K92,B73:K73,B54:K54,B35:K35,B16:K16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4073,140 +4028,140 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table68" displayName="Table68" ref="A99:K114" totalsRowShown="0" headerRowDxfId="114" headerRowBorderDxfId="112" tableBorderDxfId="113">
-  <autoFilter ref="A99:K114" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table68" displayName="Table68" ref="A99:K114" totalsRowShown="0" headerRowDxfId="114" headerRowBorderDxfId="113" tableBorderDxfId="112">
+  <autoFilter ref="A99:K114"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Josh's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="jMonkeyEngine" dataDxfId="111"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="libGDX" dataDxfId="110"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="TEAMMATES" dataDxfId="109"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="JUnit 4" dataDxfId="108"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Activiti" dataDxfId="107"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Kore" dataDxfId="106"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="MyCollab" dataDxfId="105"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="BioJava" dataDxfId="104"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Cryptomator" dataDxfId="103"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Java Google Maps" dataDxfId="102"/>
+    <tableColumn id="1" name="Josh's Projects"/>
+    <tableColumn id="2" name="jMonkeyEngine" dataDxfId="111"/>
+    <tableColumn id="4" name="libGDX" dataDxfId="110"/>
+    <tableColumn id="5" name="TEAMMATES" dataDxfId="109"/>
+    <tableColumn id="6" name="JUnit 4" dataDxfId="108"/>
+    <tableColumn id="7" name="Activiti" dataDxfId="107"/>
+    <tableColumn id="8" name="Kore" dataDxfId="106"/>
+    <tableColumn id="9" name="MyCollab" dataDxfId="105"/>
+    <tableColumn id="10" name="BioJava" dataDxfId="104"/>
+    <tableColumn id="11" name="Cryptomator" dataDxfId="103"/>
+    <tableColumn id="12" name="Java Google Maps" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table79" displayName="Table79" ref="A80:K95" totalsRowShown="0">
-  <autoFilter ref="A80:K95" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table79" displayName="Table79" ref="A80:K95" totalsRowShown="0">
+  <autoFilter ref="A80:K95"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Amy's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Shimmer"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Applozic"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Ribot"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="PocketHub"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="ownCloud"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Slide"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="OpenLauncher"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="Activity Tracking/Location Sharing App"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="Note App"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Plaid App"/>
+    <tableColumn id="1" name="Amy's Projects"/>
+    <tableColumn id="2" name="Shimmer"/>
+    <tableColumn id="4" name="Applozic"/>
+    <tableColumn id="5" name="Ribot"/>
+    <tableColumn id="6" name="PocketHub"/>
+    <tableColumn id="7" name="ownCloud"/>
+    <tableColumn id="8" name="Slide"/>
+    <tableColumn id="9" name="OpenLauncher"/>
+    <tableColumn id="10" name="Activity Tracking/Location Sharing App"/>
+    <tableColumn id="11" name="Note App"/>
+    <tableColumn id="12" name="Plaid App"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table76" displayName="Table76" ref="A4:K19" totalsRowShown="0" headerRowDxfId="101">
-  <autoFilter ref="A4:K19" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table76" displayName="Table76" ref="A4:K19" totalsRowShown="0" headerRowDxfId="101">
+  <autoFilter ref="A4:K19"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Tony's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Hadoop BAM (genomics)"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Chemistry DK."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Jannovar for VCF"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Varsim"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Cancer Registry cgritt"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="openCGA"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="intermine"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Caleydo"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="IGV"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="Irida-dev"/>
+    <tableColumn id="1" name="Tony's Projects"/>
+    <tableColumn id="2" name="Hadoop BAM (genomics)"/>
+    <tableColumn id="4" name="Chemistry DK."/>
+    <tableColumn id="5" name="Jannovar for VCF"/>
+    <tableColumn id="6" name="Varsim"/>
+    <tableColumn id="7" name="Cancer Registry cgritt"/>
+    <tableColumn id="8" name="openCGA"/>
+    <tableColumn id="9" name="intermine"/>
+    <tableColumn id="10" name="Caleydo"/>
+    <tableColumn id="11" name="IGV"/>
+    <tableColumn id="12" name="Irida-dev"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table767" displayName="Table767" ref="A23:K38" totalsRowShown="0">
-  <autoFilter ref="A23:K38" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table767" displayName="Table767" ref="A23:K38" totalsRowShown="0">
+  <autoFilter ref="A23:K38"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Wilfredo's Projects "/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Dungeon"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Game Engine"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Magarena"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Xmage"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Martian Run"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Mindustry"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="PretendYoureXyzzy"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Seventh"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="Stendhal"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="Terasology"/>
+    <tableColumn id="1" name="Wilfredo's Projects "/>
+    <tableColumn id="2" name="Dungeon"/>
+    <tableColumn id="4" name="Game Engine"/>
+    <tableColumn id="5" name="Magarena"/>
+    <tableColumn id="6" name="Xmage"/>
+    <tableColumn id="7" name="Martian Run"/>
+    <tableColumn id="8" name="Mindustry"/>
+    <tableColumn id="9" name="PretendYoureXyzzy"/>
+    <tableColumn id="10" name="Seventh"/>
+    <tableColumn id="11" name="Stendhal"/>
+    <tableColumn id="12" name="Terasology"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table7679" displayName="Table7679" ref="A42:K57" totalsRowShown="0">
-  <autoFilter ref="A42:K57" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table7679" displayName="Table7679" ref="A42:K57" totalsRowShown="0">
+  <autoFilter ref="A42:K57"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Logan's Projects "/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Crawler4j"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Incibator Dubbo"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="KillBill"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Open Refine"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Stage Monitor"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Graph Hopper"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="h20.io"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Omni Notes"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="pinpoint"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="openFire"/>
+    <tableColumn id="1" name="Logan's Projects "/>
+    <tableColumn id="2" name="Crawler4j"/>
+    <tableColumn id="4" name="Incibator Dubbo"/>
+    <tableColumn id="5" name="KillBill"/>
+    <tableColumn id="6" name="Open Refine"/>
+    <tableColumn id="7" name="Stage Monitor"/>
+    <tableColumn id="8" name="Graph Hopper"/>
+    <tableColumn id="9" name="h20.io"/>
+    <tableColumn id="10" name="Omni Notes"/>
+    <tableColumn id="11" name="pinpoint"/>
+    <tableColumn id="12" name="openFire"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table767910" displayName="Table767910" ref="A61:K76" totalsRowShown="0" headerRowDxfId="100">
-  <autoFilter ref="A61:K76" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table767910" displayName="Table767910" ref="A61:K76" totalsRowShown="0" headerRowDxfId="100">
+  <autoFilter ref="A61:K76"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Sim's Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Quartz Scheduler" dataDxfId="99"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Open EMRConect"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Wallet"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Secure Banking System"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Calendar System"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Time4J"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Voj "/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Core Flight Systm(CFS) and data Dictionary(CCDD) Utility"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Dert"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Hyper realistic zombie"/>
+    <tableColumn id="1" name="Sim's Projects"/>
+    <tableColumn id="2" name="Quartz Scheduler" dataDxfId="99"/>
+    <tableColumn id="4" name="Open EMRConect"/>
+    <tableColumn id="5" name="Wallet"/>
+    <tableColumn id="6" name="Secure Banking System"/>
+    <tableColumn id="7" name="Calendar System"/>
+    <tableColumn id="8" name="Time4J"/>
+    <tableColumn id="9" name="Voj "/>
+    <tableColumn id="10" name="Core Flight Systm(CFS) and data Dictionary(CCDD) Utility"/>
+    <tableColumn id="11" name="Dert"/>
+    <tableColumn id="12" name="Hyper realistic zombie"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table511" displayName="Table511" ref="A158:K172" totalsRowShown="0" headerRowDxfId="98" headerRowBorderDxfId="96" tableBorderDxfId="97">
-  <autoFilter ref="A158:K172" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table511" displayName="Table511" ref="A158:K172" totalsRowShown="0" headerRowDxfId="98" headerRowBorderDxfId="97" tableBorderDxfId="96">
+  <autoFilter ref="A158:K172"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Robert’s Projects"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Jpacman Framework" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="seventh" dataDxfId="94"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Snake" dataDxfId="93"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Java String Similarity" dataDxfId="92"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="LeetCode Sol Res" dataDxfId="91"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Game of Life in Java" dataDxfId="90"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="EduMIPS64" dataDxfId="89"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="ATM Simulator" dataDxfId="88"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="RinSim" dataDxfId="87"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Mathematics" dataDxfId="86"/>
+    <tableColumn id="1" name="Robert’s Projects"/>
+    <tableColumn id="2" name="Jpacman Framework" dataDxfId="95"/>
+    <tableColumn id="4" name="seventh" dataDxfId="94"/>
+    <tableColumn id="5" name="Snake" dataDxfId="93"/>
+    <tableColumn id="6" name="Java String Similarity" dataDxfId="92"/>
+    <tableColumn id="7" name="LeetCode Sol Res" dataDxfId="91"/>
+    <tableColumn id="8" name="Game of Life in Java" dataDxfId="90"/>
+    <tableColumn id="9" name="EduMIPS64" dataDxfId="89"/>
+    <tableColumn id="10" name="ATM Simulator" dataDxfId="88"/>
+    <tableColumn id="11" name="RinSim" dataDxfId="87"/>
+    <tableColumn id="12" name="Mathematics" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4474,36 +4429,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U200"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:U199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F174" zoomScale="58" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="Q196" sqref="Q196:Q199"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="82" workbookViewId="0">
+      <selection activeCell="A183" sqref="A183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="20.875" customWidth="1"/>
-    <col min="9" max="9" width="20.25" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="15.125" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" customWidth="1"/>
     <col min="12" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="20" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="39.950000000000003" customHeight="1">
+    <row r="2" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4516,7 +4463,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4529,45 +4476,48 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1"/>
+      <c r="M4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>11</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -4601,9 +4551,9 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -4640,9 +4590,9 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -4679,9 +4629,9 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
         <v>34</v>
@@ -4715,9 +4665,9 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>67</v>
@@ -4751,9 +4701,9 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>47</v>
@@ -4787,10 +4737,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>0</v>
       </c>
@@ -4827,9 +4774,9 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -4867,9 +4814,9 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -4907,9 +4854,9 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="15.75">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -4944,33 +4891,33 @@
         <v>8</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="55" t="s">
+      <c r="M14" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="N14" s="55"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.75">
-      <c r="A15" t="s">
+      <c r="O15" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="M15" s="41" t="s">
+      <c r="P15" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="48" t="s">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>26</v>
-      </c>
-      <c r="O15" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="P15" s="52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15.75">
-      <c r="A16" t="s">
-        <v>29</v>
       </c>
       <c r="B16">
         <f>B5/SUM(B5:B14)*100</f>
@@ -5026,9 +4973,9 @@
       </c>
       <c r="P16" s="53"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <f>B7/SUM(B5:B14)*100</f>
@@ -5084,9 +5031,9 @@
       </c>
       <c r="P17" s="45"/>
     </row>
-    <row r="18" spans="1:18" ht="15.95" customHeight="1">
+    <row r="18" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <f>B6/SUM(B5:B14)*100</f>
@@ -5142,9 +5089,9 @@
       </c>
       <c r="P18" s="45"/>
     </row>
-    <row r="19" spans="1:18" ht="15.95" customHeight="1">
+    <row r="19" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <f>SUM(B16:B18)</f>
@@ -5200,62 +5147,62 @@
       </c>
       <c r="P19" s="46"/>
     </row>
-    <row r="20" spans="1:18" ht="15.95" customHeight="1">
+    <row r="20" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M20" s="54"/>
       <c r="N20" s="54"/>
       <c r="O20" s="54"/>
       <c r="P20" s="23"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E23" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
+      <c r="F23" t="s">
         <v>35</v>
       </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
         <v>36</v>
       </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
         <v>37</v>
       </c>
-      <c r="F23" t="s">
+      <c r="I23" t="s">
         <v>38</v>
       </c>
-      <c r="G23" t="s">
+      <c r="J23" t="s">
         <v>39</v>
       </c>
-      <c r="H23" t="s">
+      <c r="K23" t="s">
         <v>40</v>
-      </c>
-      <c r="I23" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" t="s">
-        <v>42</v>
-      </c>
-      <c r="K23" t="s">
-        <v>43</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -5290,9 +5237,9 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -5327,9 +5274,9 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>15</v>
@@ -5364,9 +5311,9 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>301</v>
@@ -5401,9 +5348,9 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B28">
         <v>726</v>
@@ -5438,125 +5385,122 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>18</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="5"/>
-    </row>
-    <row r="30" spans="1:18">
-      <c r="A30" t="s">
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>19</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="5"/>
-    </row>
-    <row r="31" spans="1:18">
-      <c r="A31" t="s">
+      <c r="M33" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="5"/>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q32" s="5"/>
-    </row>
-    <row r="33" spans="1:18" ht="15.75">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="M33" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="N33" s="55"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="55"/>
+      <c r="N33" s="66"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
     </row>
-    <row r="34" spans="1:18" ht="15.75">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="O34" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="M34" s="41" t="s">
+      <c r="P34" s="52" t="s">
         <v>25</v>
-      </c>
-      <c r="N34" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="O34" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="P34" s="52" t="s">
-        <v>28</v>
       </c>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
     </row>
-    <row r="35" spans="1:18" ht="15.75">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B35">
         <f>B24/SUM(B24:B33)*100</f>
@@ -5612,9 +5556,9 @@
       </c>
       <c r="P35" s="53"/>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B36">
         <f>B26/SUM(B24:B33)*100</f>
@@ -5670,9 +5614,9 @@
       </c>
       <c r="P36" s="45"/>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B37">
         <f>B25/SUM(B24:B33)*100</f>
@@ -5728,9 +5672,9 @@
       </c>
       <c r="P37" s="45"/>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B38">
         <f>SUM(B35:B37)</f>
@@ -5786,56 +5730,56 @@
       </c>
       <c r="P38" s="46"/>
     </row>
-    <row r="39" spans="1:18" ht="15.75">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M39" s="54"/>
       <c r="N39" s="54"/>
       <c r="O39" s="54"/>
       <c r="P39" s="23"/>
     </row>
-    <row r="40" spans="1:18" ht="15.75">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M40" s="54"/>
       <c r="N40" s="54"/>
       <c r="O40" s="54"/>
       <c r="P40" s="23"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="E42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" t="s">
+      <c r="F42" t="s">
         <v>46</v>
       </c>
-      <c r="D42" t="s">
+      <c r="G42" t="s">
         <v>47</v>
       </c>
-      <c r="E42" t="s">
+      <c r="H42" t="s">
         <v>48</v>
       </c>
-      <c r="F42" t="s">
+      <c r="I42" t="s">
         <v>49</v>
       </c>
-      <c r="G42" t="s">
+      <c r="J42" t="s">
         <v>50</v>
       </c>
-      <c r="H42" t="s">
+      <c r="K42" t="s">
         <v>51</v>
       </c>
-      <c r="I42" t="s">
-        <v>52</v>
-      </c>
-      <c r="J42" t="s">
-        <v>53</v>
-      </c>
-      <c r="K42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18">
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -5868,9 +5812,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -5903,9 +5847,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -5938,9 +5882,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B46">
         <v>71</v>
@@ -5973,9 +5917,9 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47">
         <v>256</v>
@@ -6008,9 +5952,9 @@
         <v>4809</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B48">
         <v>48</v>
@@ -6043,10 +5987,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
-      <c r="A49" t="s">
-        <v>19</v>
-      </c>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>0</v>
       </c>
@@ -6078,9 +6019,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -6113,9 +6054,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -6148,9 +6089,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="15.75">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -6182,33 +6123,33 @@
       <c r="K52">
         <v>1</v>
       </c>
-      <c r="M52" s="55" t="s">
+      <c r="M52" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="N52" s="66"/>
+      <c r="O52" s="66"/>
+      <c r="P52" s="66"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N53" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="N52" s="55"/>
-      <c r="O52" s="55"/>
-      <c r="P52" s="55"/>
-    </row>
-    <row r="53" spans="1:16" ht="15.75">
-      <c r="A53" t="s">
+      <c r="O53" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="M53" s="41" t="s">
+      <c r="P53" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N53" s="48" t="s">
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>26</v>
-      </c>
-      <c r="O53" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="P53" s="52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="15.75">
-      <c r="A54" t="s">
-        <v>29</v>
       </c>
       <c r="B54">
         <f>B43/SUM(B43:B52)</f>
@@ -6264,9 +6205,9 @@
       </c>
       <c r="P54" s="53"/>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B55">
         <f>B45/SUM(B43:B52)*100</f>
@@ -6322,9 +6263,9 @@
       </c>
       <c r="P55" s="45"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B56">
         <f>B44/SUM(B43:B52)*100</f>
@@ -6380,9 +6321,9 @@
       </c>
       <c r="P56" s="45"/>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B57">
         <f>SUM(B54:B56)</f>
@@ -6438,57 +6379,57 @@
       </c>
       <c r="P57" s="46"/>
     </row>
-    <row r="58" spans="1:16" ht="15.75">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="M58" s="54"/>
       <c r="N58" s="54"/>
       <c r="O58" s="54"/>
       <c r="P58" s="23"/>
     </row>
-    <row r="59" spans="1:16" ht="15.75">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="M59" s="54"/>
       <c r="N59" s="54"/>
       <c r="O59" s="54"/>
       <c r="P59" s="23"/>
     </row>
-    <row r="61" spans="1:16" ht="80.099999999999994">
+    <row r="61" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="E61" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="F61" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="G61" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="H61" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="I61" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="J61" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H61" s="6" t="s">
+      <c r="K61" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I61" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="K61" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B62" s="5">
         <v>71</v>
@@ -6521,9 +6462,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B63" s="5">
         <v>0</v>
@@ -6556,9 +6497,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B64" s="5">
         <v>0</v>
@@ -6591,9 +6532,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B65" s="5">
         <v>459</v>
@@ -6626,9 +6567,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B66" s="5">
         <v>1181</v>
@@ -6661,9 +6602,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B67" s="5">
         <v>517</v>
@@ -6696,10 +6637,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
-      <c r="A68" s="5" t="s">
-        <v>68</v>
-      </c>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A68" s="5"/>
       <c r="B68" s="5">
         <v>0</v>
       </c>
@@ -6731,51 +6670,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" s="5"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="M71" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B69" s="5"/>
-    </row>
-    <row r="70" spans="1:16" ht="15.75">
-      <c r="A70" t="s">
+      <c r="N71" s="66"/>
+      <c r="O71" s="66"/>
+      <c r="P71" s="66"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>21</v>
-      </c>
-      <c r="B70" s="5"/>
-    </row>
-    <row r="71" spans="1:16" ht="15.75">
-      <c r="A71" t="s">
-        <v>22</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="M71" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="N71" s="55"/>
-      <c r="O71" s="55"/>
-      <c r="P71" s="55"/>
-    </row>
-    <row r="72" spans="1:16" ht="15.75">
-      <c r="A72" t="s">
-        <v>24</v>
       </c>
       <c r="B72" s="5"/>
       <c r="M72" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N72" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="O72" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P72" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N72" s="48" t="s">
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>26</v>
-      </c>
-      <c r="O72" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="P72" s="52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" ht="15.75">
-      <c r="A73" t="s">
-        <v>29</v>
       </c>
       <c r="B73" s="5">
         <f>B62/SUM(B62:B71)*100</f>
@@ -6832,9 +6771,9 @@
       </c>
       <c r="P73" s="53"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B74" s="5">
         <f>B64/SUM(B62:B71)*100</f>
@@ -6891,9 +6830,9 @@
       </c>
       <c r="P74" s="45"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B75">
         <f>B63/SUM(B62:B71)*100</f>
@@ -6949,9 +6888,9 @@
       </c>
       <c r="P75" s="45"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B76">
         <f>SUM(B73:B75)</f>
@@ -7007,54 +6946,54 @@
       </c>
       <c r="P76" s="46"/>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C80" t="s">
+        <v>67</v>
+      </c>
+      <c r="D80" t="s">
+        <v>68</v>
+      </c>
+      <c r="E80" t="s">
         <v>69</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="F80" t="s">
         <v>70</v>
       </c>
-      <c r="C80" t="s">
+      <c r="G80" t="s">
         <v>71</v>
       </c>
-      <c r="D80" t="s">
+      <c r="H80" t="s">
         <v>72</v>
       </c>
-      <c r="E80" t="s">
+      <c r="I80" t="s">
         <v>73</v>
       </c>
-      <c r="F80" t="s">
+      <c r="J80" t="s">
         <v>74</v>
       </c>
-      <c r="G80" t="s">
+      <c r="K80" t="s">
         <v>75</v>
       </c>
-      <c r="H80" t="s">
-        <v>76</v>
-      </c>
-      <c r="I80" t="s">
-        <v>77</v>
-      </c>
-      <c r="J80" t="s">
-        <v>78</v>
-      </c>
-      <c r="K80" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16">
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -7087,9 +7026,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -7122,9 +7061,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -7157,9 +7096,9 @@
         <v>312</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B84">
         <v>2</v>
@@ -7192,9 +7131,9 @@
         <v>318</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B85">
         <v>71</v>
@@ -7227,9 +7166,9 @@
         <v>896</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B86">
         <v>11</v>
@@ -7262,10 +7201,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
-      <c r="A87" t="s">
-        <v>19</v>
-      </c>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B87">
         <v>0</v>
       </c>
@@ -7297,9 +7233,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -7332,9 +7268,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -7367,9 +7303,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="15.75">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -7401,33 +7337,33 @@
       <c r="K90">
         <v>1</v>
       </c>
-      <c r="M90" s="55" t="s">
+      <c r="M90" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="N90" s="66"/>
+      <c r="O90" s="66"/>
+      <c r="P90" s="66"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>21</v>
+      </c>
+      <c r="M91" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N91" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="N90" s="55"/>
-      <c r="O90" s="55"/>
-      <c r="P90" s="55"/>
-    </row>
-    <row r="91" spans="1:16" ht="15.75">
-      <c r="A91" t="s">
+      <c r="O91" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="M91" s="41" t="s">
+      <c r="P91" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N91" s="48" t="s">
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>26</v>
-      </c>
-      <c r="O91" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="P91" s="52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" ht="15.75">
-      <c r="A92" t="s">
-        <v>29</v>
       </c>
       <c r="B92">
         <f>(B81/SUM(B81:B90)) * 100</f>
@@ -7483,9 +7419,9 @@
       </c>
       <c r="P92" s="53"/>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B93">
         <f>(B82/SUM(B81:B90)) * 100</f>
@@ -7541,9 +7477,9 @@
       </c>
       <c r="P93" s="45"/>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B94">
         <f>(B83/SUM(B81:B90)) * 100</f>
@@ -7599,9 +7535,9 @@
       </c>
       <c r="P94" s="45"/>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B95">
         <f>SUM(B92:B94)</f>
@@ -7657,58 +7593,58 @@
       </c>
       <c r="P95" s="46"/>
     </row>
-    <row r="96" spans="1:16" ht="15.75">
-      <c r="A96" s="59"/>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A96" s="55"/>
       <c r="M96" s="54"/>
       <c r="N96" s="54"/>
       <c r="O96" s="54"/>
       <c r="P96" s="23"/>
     </row>
-    <row r="97" spans="1:16" ht="15.75">
-      <c r="A97" s="59"/>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A97" s="55"/>
       <c r="M97" s="54"/>
       <c r="N97" s="54"/>
       <c r="O97" s="54"/>
       <c r="P97" s="23"/>
     </row>
-    <row r="99" spans="1:16" ht="17.100000000000001" thickBot="1">
+    <row r="99" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B99" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D99" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E99" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B99" s="20" t="s">
+      <c r="F99" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C99" s="21" t="s">
+      <c r="G99" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D99" s="21" t="s">
+      <c r="H99" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="E99" s="21" t="s">
+      <c r="I99" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="F99" s="21" t="s">
+      <c r="J99" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="G99" s="21" t="s">
+      <c r="K99" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="H99" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="I99" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="J99" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="K99" s="22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16">
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B100" s="11">
         <v>789</v>
@@ -7741,9 +7677,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B101" s="11">
         <v>0</v>
@@ -7776,9 +7712,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B102" s="11">
         <v>79</v>
@@ -7811,9 +7747,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B103" s="11">
         <v>1686</v>
@@ -7846,9 +7782,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B104" s="11">
         <v>13134</v>
@@ -7881,9 +7817,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B105" s="11">
         <v>2150</v>
@@ -7916,10 +7852,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
-      <c r="A106" t="s">
-        <v>19</v>
-      </c>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B106" s="11">
         <v>0</v>
       </c>
@@ -7951,9 +7884,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B107" s="11">
         <v>3</v>
@@ -7986,9 +7919,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B108" s="11">
         <v>0</v>
@@ -8021,9 +7954,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="15.75">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B109" s="11">
         <v>8</v>
@@ -8055,16 +7988,16 @@
       <c r="K109" s="11">
         <v>0</v>
       </c>
-      <c r="M109" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="N109" s="55"/>
-      <c r="O109" s="55"/>
-      <c r="P109" s="55"/>
-    </row>
-    <row r="110" spans="1:16" ht="15.75">
+      <c r="M109" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="N109" s="66"/>
+      <c r="O109" s="66"/>
+      <c r="P109" s="66"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B110" s="13"/>
       <c r="C110" s="13"/>
@@ -8074,21 +8007,21 @@
       <c r="J110" s="13"/>
       <c r="K110" s="13"/>
       <c r="M110" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N110" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="O110" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P110" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N110" s="48" t="s">
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>26</v>
-      </c>
-      <c r="O110" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="P110" s="52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" ht="15.75">
-      <c r="A111" t="s">
-        <v>29</v>
       </c>
       <c r="B111" s="13">
         <f>(B100/SUM(B100:B109)) * 100</f>
@@ -8144,9 +8077,9 @@
       </c>
       <c r="P111" s="53"/>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B112" s="13">
         <f>(B101/SUM(B100:B109)) * 100</f>
@@ -8202,9 +8135,9 @@
       </c>
       <c r="P112" s="45"/>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B113" s="15">
         <f>(B102/SUM(B100:B109)) * 100</f>
@@ -8260,9 +8193,9 @@
       </c>
       <c r="P113" s="45"/>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B114" s="23">
         <f>SUM(B111:B113)</f>
@@ -8318,8 +8251,8 @@
       </c>
       <c r="P114" s="46"/>
     </row>
-    <row r="115" spans="1:16" ht="15.75">
-      <c r="A115" s="59"/>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A115" s="55"/>
       <c r="B115" s="23"/>
       <c r="C115" s="23"/>
       <c r="D115" s="23"/>
@@ -8335,8 +8268,8 @@
       <c r="O115" s="54"/>
       <c r="P115" s="23"/>
     </row>
-    <row r="116" spans="1:16" ht="15.75">
-      <c r="A116" s="59"/>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A116" s="55"/>
       <c r="B116" s="23"/>
       <c r="C116" s="23"/>
       <c r="D116" s="23"/>
@@ -8352,44 +8285,44 @@
       <c r="O116" s="54"/>
       <c r="P116" s="23"/>
     </row>
-    <row r="118" spans="1:16" ht="17.100000000000001" thickBot="1">
+    <row r="118" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B118" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C118" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D118" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E118" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B118" s="20" t="s">
+      <c r="F118" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C118" s="21" t="s">
+      <c r="G118" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="D118" s="21" t="s">
+      <c r="H118" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E118" s="21" t="s">
+      <c r="I118" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F118" s="21" t="s">
+      <c r="J118" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="G118" s="21" t="s">
+      <c r="K118" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="H118" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="I118" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="J118" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="K118" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="119" spans="1:16">
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B119" s="11">
         <v>0</v>
@@ -8422,9 +8355,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B120" s="11">
         <v>0</v>
@@ -8457,9 +8390,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B121" s="11">
         <v>0</v>
@@ -8492,9 +8425,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B122" s="11">
         <v>18</v>
@@ -8527,9 +8460,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B123" s="11">
         <v>14</v>
@@ -8562,9 +8495,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B124" s="11">
         <v>25</v>
@@ -8597,114 +8530,111 @@
         <v>180</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
-      <c r="A125" t="s">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B125" s="11">
+        <v>0</v>
+      </c>
+      <c r="C125" s="11">
+        <v>0</v>
+      </c>
+      <c r="D125" s="11">
+        <v>0</v>
+      </c>
+      <c r="E125" s="16">
+        <v>0</v>
+      </c>
+      <c r="F125" s="11">
+        <v>0</v>
+      </c>
+      <c r="G125" s="12">
+        <v>0</v>
+      </c>
+      <c r="H125" s="11">
+        <v>0</v>
+      </c>
+      <c r="I125" s="12">
+        <v>0</v>
+      </c>
+      <c r="J125" s="11">
+        <v>0</v>
+      </c>
+      <c r="K125" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>17</v>
+      </c>
+      <c r="B126" s="11">
+        <v>0</v>
+      </c>
+      <c r="C126" s="11">
+        <v>0</v>
+      </c>
+      <c r="D126" s="11">
+        <v>0</v>
+      </c>
+      <c r="E126" s="16">
+        <v>0</v>
+      </c>
+      <c r="F126" s="11">
+        <v>0</v>
+      </c>
+      <c r="G126" s="12">
+        <v>0</v>
+      </c>
+      <c r="H126" s="11">
+        <v>0</v>
+      </c>
+      <c r="I126" s="12">
+        <v>0</v>
+      </c>
+      <c r="J126" s="11">
+        <v>0</v>
+      </c>
+      <c r="K126" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>18</v>
+      </c>
+      <c r="B127" s="11">
+        <v>0</v>
+      </c>
+      <c r="C127" s="11">
+        <v>0</v>
+      </c>
+      <c r="D127" s="11">
+        <v>0</v>
+      </c>
+      <c r="E127" s="16">
+        <v>0</v>
+      </c>
+      <c r="F127" s="11">
+        <v>0</v>
+      </c>
+      <c r="G127" s="12">
+        <v>0</v>
+      </c>
+      <c r="H127" s="11">
+        <v>0</v>
+      </c>
+      <c r="I127" s="12">
+        <v>0</v>
+      </c>
+      <c r="J127" s="11">
+        <v>0</v>
+      </c>
+      <c r="K127" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>19</v>
-      </c>
-      <c r="B125" s="11">
-        <v>0</v>
-      </c>
-      <c r="C125" s="11">
-        <v>0</v>
-      </c>
-      <c r="D125" s="11">
-        <v>0</v>
-      </c>
-      <c r="E125" s="16">
-        <v>0</v>
-      </c>
-      <c r="F125" s="11">
-        <v>0</v>
-      </c>
-      <c r="G125" s="12">
-        <v>0</v>
-      </c>
-      <c r="H125" s="11">
-        <v>0</v>
-      </c>
-      <c r="I125" s="12">
-        <v>0</v>
-      </c>
-      <c r="J125" s="11">
-        <v>0</v>
-      </c>
-      <c r="K125" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:16">
-      <c r="A126" t="s">
-        <v>20</v>
-      </c>
-      <c r="B126" s="11">
-        <v>0</v>
-      </c>
-      <c r="C126" s="11">
-        <v>0</v>
-      </c>
-      <c r="D126" s="11">
-        <v>0</v>
-      </c>
-      <c r="E126" s="16">
-        <v>0</v>
-      </c>
-      <c r="F126" s="11">
-        <v>0</v>
-      </c>
-      <c r="G126" s="12">
-        <v>0</v>
-      </c>
-      <c r="H126" s="11">
-        <v>0</v>
-      </c>
-      <c r="I126" s="12">
-        <v>0</v>
-      </c>
-      <c r="J126" s="11">
-        <v>0</v>
-      </c>
-      <c r="K126" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16">
-      <c r="A127" t="s">
-        <v>21</v>
-      </c>
-      <c r="B127" s="11">
-        <v>0</v>
-      </c>
-      <c r="C127" s="11">
-        <v>0</v>
-      </c>
-      <c r="D127" s="11">
-        <v>0</v>
-      </c>
-      <c r="E127" s="16">
-        <v>0</v>
-      </c>
-      <c r="F127" s="11">
-        <v>0</v>
-      </c>
-      <c r="G127" s="12">
-        <v>0</v>
-      </c>
-      <c r="H127" s="11">
-        <v>0</v>
-      </c>
-      <c r="I127" s="12">
-        <v>0</v>
-      </c>
-      <c r="J127" s="11">
-        <v>0</v>
-      </c>
-      <c r="K127" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" ht="15.75">
-      <c r="A128" t="s">
-        <v>22</v>
       </c>
       <c r="B128" s="11">
         <v>0</v>
@@ -8736,16 +8666,16 @@
       <c r="K128" s="11">
         <v>0</v>
       </c>
-      <c r="M128" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="N128" s="55"/>
-      <c r="O128" s="55"/>
-      <c r="P128" s="55"/>
-    </row>
-    <row r="129" spans="1:17" ht="15.75">
+      <c r="M128" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="N128" s="66"/>
+      <c r="O128" s="66"/>
+      <c r="P128" s="66"/>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B129" s="13">
         <v>15</v>
@@ -8778,21 +8708,21 @@
         <v>103</v>
       </c>
       <c r="M129" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N129" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="O129" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P129" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="N129" s="48" t="s">
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>26</v>
-      </c>
-      <c r="O129" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="P129" s="52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" ht="15.75">
-      <c r="A130" t="s">
-        <v>29</v>
       </c>
       <c r="B130" s="13">
         <f>B119/SUM(B119:B128)*100</f>
@@ -8848,9 +8778,9 @@
       </c>
       <c r="P130" s="53"/>
     </row>
-    <row r="131" spans="1:17">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B131" s="13">
         <f>B120/SUM(B119:B128)*100</f>
@@ -8906,9 +8836,9 @@
       </c>
       <c r="P131" s="45"/>
     </row>
-    <row r="132" spans="1:17">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B132" s="13">
         <f>B121/SUM(B119:B128)*100</f>
@@ -8964,9 +8894,9 @@
       </c>
       <c r="P132" s="45"/>
     </row>
-    <row r="133" spans="1:17">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B133" s="15">
         <f>SUM(B130:B132)</f>
@@ -9022,8 +8952,8 @@
       </c>
       <c r="P133" s="46"/>
     </row>
-    <row r="134" spans="1:17" ht="15.75">
-      <c r="A134" s="59"/>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A134" s="55"/>
       <c r="B134" s="23"/>
       <c r="C134" s="23"/>
       <c r="D134" s="23"/>
@@ -9039,8 +8969,8 @@
       <c r="O134" s="54"/>
       <c r="P134" s="23"/>
     </row>
-    <row r="135" spans="1:17" ht="15.75">
-      <c r="A135" s="59"/>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A135" s="55"/>
       <c r="B135" s="23"/>
       <c r="C135" s="23"/>
       <c r="D135" s="23"/>
@@ -9056,100 +8986,100 @@
       <c r="O135" s="54"/>
       <c r="P135" s="23"/>
     </row>
-    <row r="137" spans="1:17" ht="17.100000000000001" thickBot="1">
+    <row r="137" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B137" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C137" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D137" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E137" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B137" s="20" t="s">
+      <c r="F137" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C137" s="24" t="s">
+      <c r="G137" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D137" s="21" t="s">
+      <c r="H137" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E137" s="21" t="s">
+      <c r="I137" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="F137" s="21" t="s">
+      <c r="J137" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="G137" s="21" t="s">
+      <c r="K137" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="H137" s="21" t="s">
+      <c r="L137" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="I137" s="21" t="s">
+      <c r="M137" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="J137" s="21" t="s">
+      <c r="N137" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="K137" s="21" t="s">
+      <c r="O137" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="L137" s="22" t="s">
+      <c r="P137" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="M137" s="19" t="s">
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="N137" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="O137" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="P137" s="25" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="138" spans="1:17">
-      <c r="A138" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
       <c r="D138" s="11"/>
       <c r="E138" s="26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F138" s="27" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G138" s="26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H138" s="28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I138" s="11"/>
       <c r="J138" s="12"/>
       <c r="K138" s="26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L138" s="26" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="M138" s="29" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="N138" s="26" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O138" s="26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="P138" s="30" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Q138" s="31"/>
     </row>
-    <row r="139" spans="1:17">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B139" s="11">
         <v>4</v>
@@ -9197,9 +9127,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:17">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B140" s="11">
         <v>0</v>
@@ -9247,9 +9177,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:17">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B141" s="11">
         <v>4</v>
@@ -9297,9 +9227,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="142" spans="1:17">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B142" s="11">
         <v>58</v>
@@ -9347,9 +9277,9 @@
         <v>545</v>
       </c>
     </row>
-    <row r="143" spans="1:17">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B143" s="11">
         <v>48</v>
@@ -9397,9 +9327,9 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="144" spans="1:17">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B144" s="11">
         <v>38</v>
@@ -9447,10 +9377,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="145" spans="1:21">
-      <c r="A145" t="s">
-        <v>19</v>
-      </c>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B145" s="11">
         <v>0</v>
       </c>
@@ -9497,9 +9424,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="15.75">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B146" s="11">
         <v>0</v>
@@ -9547,9 +9474,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="15.75">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B147" s="11">
         <v>0</v>
@@ -9597,9 +9524,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="15.95" customHeight="1">
+    <row r="148" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B148" s="13">
         <v>0</v>
@@ -9646,16 +9573,16 @@
       <c r="P148" s="33">
         <v>14</v>
       </c>
-      <c r="R148" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="S148" s="55"/>
-      <c r="T148" s="55"/>
-      <c r="U148" s="55"/>
-    </row>
-    <row r="149" spans="1:21" ht="15.75">
+      <c r="R148" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="S148" s="66"/>
+      <c r="T148" s="66"/>
+      <c r="U148" s="66"/>
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B149" s="13"/>
       <c r="C149" s="13">
@@ -9691,21 +9618,21 @@
       </c>
       <c r="P149" s="33"/>
       <c r="R149" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="S149" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="T149" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="U149" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="S149" s="48" t="s">
+    </row>
+    <row r="150" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>26</v>
-      </c>
-      <c r="T149" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="U149" s="52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="150" spans="1:21" ht="15.75">
-      <c r="A150" t="s">
-        <v>29</v>
       </c>
       <c r="B150" s="13">
         <f>(B139/SUM(B139:B148)) * 100</f>
@@ -9781,9 +9708,9 @@
       </c>
       <c r="U150" s="53"/>
     </row>
-    <row r="151" spans="1:21" ht="15.75">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B151" s="13">
         <f>(B141/SUM(B139:B148)) * 100</f>
@@ -9859,9 +9786,9 @@
       </c>
       <c r="U151" s="45"/>
     </row>
-    <row r="152" spans="1:21" ht="17.100000000000001" thickBot="1">
+    <row r="152" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A152" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B152" s="15">
         <f>(B140/SUM(B139:B148)) * 100</f>
@@ -9937,9 +9864,9 @@
       </c>
       <c r="U152" s="45"/>
     </row>
-    <row r="153" spans="1:21" ht="17.100000000000001" thickBot="1">
+    <row r="153" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B153" s="8">
         <f>SUM(B150:B152)</f>
@@ -10015,7 +9942,7 @@
       </c>
       <c r="U153" s="46"/>
     </row>
-    <row r="154" spans="1:21">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B154" s="11"/>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
@@ -10031,7 +9958,7 @@
       <c r="O154" s="11"/>
       <c r="P154" s="32"/>
     </row>
-    <row r="155" spans="1:21" ht="15.75">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B155" s="54"/>
       <c r="C155" s="54"/>
       <c r="D155" s="54"/>
@@ -10047,7 +9974,7 @@
       <c r="O155" s="54"/>
       <c r="P155" s="54"/>
     </row>
-    <row r="156" spans="1:21" ht="15.75">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B156" s="54"/>
       <c r="C156" s="54"/>
       <c r="D156" s="54"/>
@@ -10063,45 +9990,44 @@
       <c r="O156" s="54"/>
       <c r="P156" s="54"/>
     </row>
-    <row r="157" spans="1:21" ht="15.75"/>
-    <row r="158" spans="1:21" ht="15.75">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E158" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="F158" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="G158" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="H158" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E158" s="1" t="s">
+      <c r="I158" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="J158" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G158" s="1" t="s">
+      <c r="K158" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H158" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I158" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J158" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K158" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="159" spans="1:21" ht="15.75">
+    </row>
+    <row r="159" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B159">
         <v>8</v>
@@ -10134,9 +10060,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="15.75">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -10169,9 +10095,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:18" ht="15.75">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -10204,9 +10130,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:18" ht="15.75">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B162">
         <v>51</v>
@@ -10239,9 +10165,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:18" ht="15.75">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B163">
         <v>182</v>
@@ -10274,9 +10200,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="164" spans="1:18" ht="15.75">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B164">
         <v>93</v>
@@ -10309,10 +10235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:18" ht="15.75">
-      <c r="A165" t="s">
-        <v>68</v>
-      </c>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B165">
         <v>0</v>
       </c>
@@ -10344,9 +10267,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:18" ht="15.75">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -10379,9 +10302,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:18" ht="15.75">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -10413,16 +10336,16 @@
       <c r="K167">
         <v>0</v>
       </c>
-      <c r="M167" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="N167" s="57"/>
-      <c r="O167" s="57"/>
-      <c r="P167" s="58"/>
-    </row>
-    <row r="168" spans="1:18" ht="15.75">
+      <c r="M167" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="N167" s="61"/>
+      <c r="O167" s="61"/>
+      <c r="P167" s="62"/>
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B168">
         <v>1</v>
@@ -10455,22 +10378,22 @@
         <v>0</v>
       </c>
       <c r="M168" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N168" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O168" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="P168" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="N168" s="39" t="s">
+      <c r="R168" s="38"/>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A169" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="O168" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="P168" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="R168" s="38"/>
-    </row>
-    <row r="169" spans="1:18" ht="15.75">
-      <c r="A169" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="B169">
         <f>B159/SUM(B159:B168)*100</f>
@@ -10526,9 +10449,9 @@
       </c>
       <c r="P169" s="45"/>
     </row>
-    <row r="170" spans="1:18" ht="15.75">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" s="37" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B170">
         <f>B160/SUM(B159:B168)*100</f>
@@ -10584,9 +10507,9 @@
       </c>
       <c r="P170" s="45"/>
     </row>
-    <row r="171" spans="1:18" ht="15.75">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A171" s="18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B171">
         <f>B161/SUM(B159:B168)*100</f>
@@ -10642,9 +10565,9 @@
       </c>
       <c r="P171" s="45"/>
     </row>
-    <row r="172" spans="1:18" ht="15.75">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A172" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B172">
         <f>SUM(B169:B171)</f>
@@ -10700,51 +10623,50 @@
       </c>
       <c r="P172" s="46"/>
     </row>
-    <row r="173" spans="1:18" ht="15.75">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O173" s="1"/>
       <c r="P173" s="1"/>
       <c r="Q173" s="1"/>
       <c r="R173" s="1"/>
     </row>
-    <row r="174" spans="1:18" ht="15.75"/>
-    <row r="176" spans="1:18">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>136</v>
+      </c>
+      <c r="B176" t="s">
+        <v>137</v>
+      </c>
+      <c r="C176" t="s">
+        <v>138</v>
+      </c>
+      <c r="D176" t="s">
+        <v>139</v>
+      </c>
+      <c r="E176" t="s">
         <v>140</v>
       </c>
-      <c r="B176" t="s">
+      <c r="F176" t="s">
         <v>141</v>
       </c>
-      <c r="C176" t="s">
+      <c r="G176" t="s">
         <v>142</v>
       </c>
-      <c r="D176" t="s">
+      <c r="H176" t="s">
         <v>143</v>
       </c>
-      <c r="E176" t="s">
+      <c r="I176" t="s">
         <v>144</v>
       </c>
-      <c r="F176" t="s">
+      <c r="J176" t="s">
         <v>145</v>
       </c>
-      <c r="G176" t="s">
+      <c r="K176" t="s">
         <v>146</v>
       </c>
-      <c r="H176" t="s">
-        <v>147</v>
-      </c>
-      <c r="I176" t="s">
-        <v>148</v>
-      </c>
-      <c r="J176" t="s">
-        <v>149</v>
-      </c>
-      <c r="K176" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="177" spans="1:16">
+    </row>
+    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B177">
         <v>69</v>
@@ -10777,9 +10699,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -10812,9 +10734,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B179">
         <v>91</v>
@@ -10847,9 +10769,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B180">
         <v>169</v>
@@ -10882,9 +10804,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B181">
         <v>785</v>
@@ -10917,9 +10839,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="182" spans="1:16">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B182">
         <v>258</v>
@@ -10952,10 +10874,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="183" spans="1:16">
-      <c r="A183" t="s">
-        <v>19</v>
-      </c>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B183">
         <v>0</v>
       </c>
@@ -10987,9 +10906,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -11022,9 +10941,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:16">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -11057,9 +10976,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:16" ht="15.75">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -11091,16 +11010,16 @@
       <c r="K186">
         <v>1</v>
       </c>
-      <c r="M186" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="N186" s="57"/>
-      <c r="O186" s="57"/>
-      <c r="P186" s="58"/>
-    </row>
-    <row r="187" spans="1:16" ht="15.75">
+      <c r="M186" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="N186" s="61"/>
+      <c r="O186" s="61"/>
+      <c r="P186" s="62"/>
+    </row>
+    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B187">
         <v>38</v>
@@ -11133,21 +11052,21 @@
         <v>56</v>
       </c>
       <c r="M187" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N187" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O187" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="P187" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="N187" s="39" t="s">
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
         <v>26</v>
-      </c>
-      <c r="O187" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="P187" s="44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="188" spans="1:16">
-      <c r="A188" t="s">
-        <v>29</v>
       </c>
       <c r="B188" s="13">
         <f>B177/SUM(B177:B186)*100</f>
@@ -11203,9 +11122,9 @@
       </c>
       <c r="P188" s="45"/>
     </row>
-    <row r="189" spans="1:16">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B189" s="13">
         <f>B178/SUM(B177:B186)*100</f>
@@ -11261,9 +11180,9 @@
       </c>
       <c r="P189" s="45"/>
     </row>
-    <row r="190" spans="1:16">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B190" s="13">
         <f>B179/SUM(B177:B186)*100</f>
@@ -11319,9 +11238,9 @@
       </c>
       <c r="P190" s="45"/>
     </row>
-    <row r="191" spans="1:16">
-      <c r="A191" s="60" t="s">
-        <v>32</v>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A191" s="56" t="s">
+        <v>29</v>
       </c>
       <c r="B191" s="13">
         <f>SUM(B188:B190)</f>
@@ -11377,36 +11296,35 @@
       </c>
       <c r="P191" s="46"/>
     </row>
-    <row r="193" spans="12:17" ht="15.75"/>
-    <row r="194" spans="12:17" ht="15.75">
-      <c r="M194" s="64" t="s">
-        <v>151</v>
-      </c>
-      <c r="N194" s="65"/>
-      <c r="O194" s="65"/>
-      <c r="P194" s="65"/>
-      <c r="Q194" s="66"/>
-    </row>
-    <row r="195" spans="12:17" ht="15.75">
-      <c r="M195" s="61" t="s">
+    <row r="194" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="M194" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="N194" s="64"/>
+      <c r="O194" s="64"/>
+      <c r="P194" s="64"/>
+      <c r="Q194" s="65"/>
+    </row>
+    <row r="195" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="M195" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="N195" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="O195" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="P195" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="N195" s="61" t="s">
+      <c r="Q195" s="57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="196" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L196" s="58" t="s">
         <v>26</v>
-      </c>
-      <c r="O195" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="P195" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q195" s="61" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="196" spans="12:17" ht="15.75">
-      <c r="L196" s="62" t="s">
-        <v>29</v>
       </c>
       <c r="M196" s="38">
         <v>15.6862745</v>
@@ -11426,9 +11344,9 @@
         <v>2.2961292895796741</v>
       </c>
     </row>
-    <row r="197" spans="12:17" ht="15.75">
-      <c r="L197" s="63" t="s">
-        <v>80</v>
+    <row r="197" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L197" s="59" t="s">
+        <v>76</v>
       </c>
       <c r="M197" s="38">
         <v>13.3359936</v>
@@ -11446,9 +11364,9 @@
         <v>0.83441732142533187</v>
       </c>
     </row>
-    <row r="198" spans="12:17" ht="15.75">
-      <c r="L198" s="62" t="s">
-        <v>81</v>
+    <row r="198" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L198" s="58" t="s">
+        <v>77</v>
       </c>
       <c r="M198" s="38">
         <v>14.2791762</v>
@@ -11468,9 +11386,9 @@
         <v>1.1588949501015127</v>
       </c>
     </row>
-    <row r="199" spans="12:17" ht="15.75">
-      <c r="L199" s="62" t="s">
-        <v>32</v>
+    <row r="199" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L199" s="58" t="s">
+        <v>29</v>
       </c>
       <c r="M199" s="38">
         <v>19.137254899999999</v>
@@ -11490,20 +11408,19 @@
         <v>4.289441561106516</v>
       </c>
     </row>
-    <row r="200" spans="12:17" ht="15.75"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="M186:P186"/>
-    <mergeCell ref="M194:Q194"/>
-    <mergeCell ref="M71:P71"/>
-    <mergeCell ref="M52:P52"/>
-    <mergeCell ref="M33:P33"/>
     <mergeCell ref="M14:P14"/>
     <mergeCell ref="M90:P90"/>
     <mergeCell ref="M167:P167"/>
     <mergeCell ref="R148:U148"/>
     <mergeCell ref="M128:P128"/>
     <mergeCell ref="M109:P109"/>
+    <mergeCell ref="M186:P186"/>
+    <mergeCell ref="M194:Q194"/>
+    <mergeCell ref="M71:P71"/>
+    <mergeCell ref="M52:P52"/>
+    <mergeCell ref="M33:P33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>